<commit_message>
Update PDS components configuration files
</commit_message>
<xml_diff>
--- a/AutoLoader/Contents/Support/PowerDistributionSystem/LV_AC_CircuitBreaker_ImportLibrary_19DX101.xlsx
+++ b/AutoLoader/Contents/Support/PowerDistributionSystem/LV_AC_CircuitBreaker_ImportLibrary_19DX101.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="MCB" sheetId="1" r:id="rId1"/>
@@ -14,8 +14,8 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">ACB!$A$2:$T$5</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MCB!$A$2:$T$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">MCCB!$A$2:$T$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MCB!$A$2:$U$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">MCCB!$A$2:$U$3</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="188">
   <si>
     <t>Trip Device</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -756,6 +756,22 @@
   </si>
   <si>
     <t>壳架规格</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>剩余电流脱扣器类型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Characteristics</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RCD Characteristics</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A;AC;B;F</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1114,30 +1130,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U34"/>
+  <dimension ref="A1:V34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.625" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.625" customWidth="1"/>
-    <col min="7" max="7" width="19.25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.625" customWidth="1"/>
-    <col min="9" max="13" width="0" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="10.625" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="10.125" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="8.625" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="13.5" hidden="1" customWidth="1"/>
-    <col min="18" max="20" width="8.625" customWidth="1"/>
+    <col min="5" max="5" width="30.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" customWidth="1"/>
+    <col min="7" max="7" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="8.6640625" customWidth="1"/>
+    <col min="10" max="14" width="8.88671875" customWidth="1"/>
+    <col min="15" max="15" width="10.6640625" customWidth="1"/>
+    <col min="16" max="16" width="10.109375" customWidth="1"/>
+    <col min="17" max="17" width="8.6640625" customWidth="1"/>
+    <col min="18" max="18" width="13.44140625" customWidth="1"/>
+    <col min="19" max="21" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" s="1" customFormat="1" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1163,46 +1179,49 @@
         <v>17</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="1" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" s="1" customFormat="1" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>33</v>
       </c>
@@ -1225,49 +1244,52 @@
         <v>154</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>16</v>
+        <v>185</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Q2" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="R2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>38</v>
       </c>
@@ -1290,14 +1312,12 @@
       <c r="H3" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="6"/>
+      <c r="J3" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="J3" s="3">
-        <v>1</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>19</v>
+      <c r="K3" s="3">
+        <v>1</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>19</v>
@@ -1305,29 +1325,32 @@
       <c r="M3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="N3" s="2">
-        <v>0.03</v>
+      <c r="N3" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="O3" s="2">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="P3" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="2">
         <v>10</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="R3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R3" s="2">
+      <c r="S3" s="2">
         <v>18</v>
       </c>
-      <c r="S3" s="2">
+      <c r="T3" s="2">
         <v>70</v>
       </c>
-      <c r="T3" s="2">
+      <c r="U3" s="2">
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>38</v>
       </c>
@@ -1350,14 +1373,12 @@
       <c r="H4" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="6"/>
+      <c r="J4" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="J4" s="3">
-        <v>1</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>19</v>
+      <c r="K4" s="3">
+        <v>1</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>19</v>
@@ -1365,29 +1386,32 @@
       <c r="M4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="N4" s="2">
-        <v>0.03</v>
+      <c r="N4" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="O4" s="2">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="P4" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="2">
         <v>10</v>
       </c>
-      <c r="Q4" s="2" t="s">
+      <c r="R4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R4" s="6">
+      <c r="S4" s="6">
         <v>18</v>
       </c>
-      <c r="S4" s="2">
+      <c r="T4" s="2">
         <v>70</v>
       </c>
-      <c r="T4" s="2">
+      <c r="U4" s="2">
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>38</v>
       </c>
@@ -1410,14 +1434,12 @@
       <c r="H5" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="6"/>
+      <c r="J5" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="J5" s="3">
-        <v>1</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>19</v>
+      <c r="K5" s="3">
+        <v>1</v>
       </c>
       <c r="L5" s="6" t="s">
         <v>19</v>
@@ -1425,29 +1447,32 @@
       <c r="M5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="N5" s="6">
-        <v>0.03</v>
+      <c r="N5" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="O5" s="6">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="P5" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="6">
         <v>10</v>
       </c>
-      <c r="Q5" s="6" t="s">
+      <c r="R5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="R5" s="6">
+      <c r="S5" s="6">
         <v>36</v>
       </c>
-      <c r="S5" s="6">
+      <c r="T5" s="6">
         <v>70</v>
       </c>
-      <c r="T5" s="6">
+      <c r="U5" s="6">
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>38</v>
       </c>
@@ -1470,14 +1495,12 @@
       <c r="H6" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="6"/>
+      <c r="J6" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="J6" s="3">
-        <v>1</v>
-      </c>
-      <c r="K6" s="6" t="s">
-        <v>19</v>
+      <c r="K6" s="3">
+        <v>1</v>
       </c>
       <c r="L6" s="6" t="s">
         <v>19</v>
@@ -1485,29 +1508,32 @@
       <c r="M6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="N6" s="6">
-        <v>0.03</v>
+      <c r="N6" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="O6" s="6">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="P6" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="6">
         <v>10</v>
       </c>
-      <c r="Q6" s="6" t="s">
+      <c r="R6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="R6" s="6">
+      <c r="S6" s="6">
         <v>36</v>
       </c>
-      <c r="S6" s="6">
+      <c r="T6" s="6">
         <v>70</v>
       </c>
-      <c r="T6" s="6">
+      <c r="U6" s="6">
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>87</v>
       </c>
@@ -1533,13 +1559,13 @@
         <v>92</v>
       </c>
       <c r="I7" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="J7" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="J7" s="3">
-        <v>1</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>85</v>
+      <c r="K7" s="3">
+        <v>1</v>
       </c>
       <c r="L7" s="6" t="s">
         <v>85</v>
@@ -1547,29 +1573,32 @@
       <c r="M7" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="N7" s="6">
-        <v>0.03</v>
+      <c r="N7" s="6" t="s">
+        <v>85</v>
       </c>
       <c r="O7" s="6">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="P7" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="6">
         <v>10</v>
       </c>
-      <c r="Q7" s="6" t="s">
+      <c r="R7" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="R7" s="6">
+      <c r="S7" s="6">
         <v>54</v>
       </c>
-      <c r="S7" s="6">
+      <c r="T7" s="6">
         <v>70</v>
       </c>
-      <c r="T7" s="6">
+      <c r="U7" s="6">
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>87</v>
       </c>
@@ -1595,13 +1624,13 @@
         <v>92</v>
       </c>
       <c r="I8" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="J8" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="J8" s="3">
-        <v>1</v>
-      </c>
-      <c r="K8" s="6" t="s">
-        <v>19</v>
+      <c r="K8" s="3">
+        <v>1</v>
       </c>
       <c r="L8" s="6" t="s">
         <v>19</v>
@@ -1609,29 +1638,32 @@
       <c r="M8" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="N8" s="6">
-        <v>0.03</v>
+      <c r="N8" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="O8" s="6">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="P8" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="6">
         <v>10</v>
       </c>
-      <c r="Q8" s="6" t="s">
+      <c r="R8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="R8" s="6">
+      <c r="S8" s="6">
         <v>36</v>
       </c>
-      <c r="S8" s="6">
+      <c r="T8" s="6">
         <v>70</v>
       </c>
-      <c r="T8" s="6">
+      <c r="U8" s="6">
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>87</v>
       </c>
@@ -1657,13 +1689,13 @@
         <v>92</v>
       </c>
       <c r="I9" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="J9" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="J9" s="3">
-        <v>1</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>85</v>
+      <c r="K9" s="3">
+        <v>1</v>
       </c>
       <c r="L9" s="6" t="s">
         <v>85</v>
@@ -1671,29 +1703,32 @@
       <c r="M9" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="N9" s="6">
-        <v>0.03</v>
+      <c r="N9" s="6" t="s">
+        <v>85</v>
       </c>
       <c r="O9" s="6">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="P9" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="6">
         <v>10</v>
       </c>
-      <c r="Q9" s="6" t="s">
+      <c r="R9" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="R9" s="6">
+      <c r="S9" s="6">
         <v>90</v>
       </c>
-      <c r="S9" s="6">
+      <c r="T9" s="6">
         <v>70</v>
       </c>
-      <c r="T9" s="6">
+      <c r="U9" s="6">
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>87</v>
       </c>
@@ -1719,13 +1754,13 @@
         <v>92</v>
       </c>
       <c r="I10" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="J10" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="J10" s="3">
-        <v>1</v>
-      </c>
-      <c r="K10" s="6" t="s">
-        <v>19</v>
+      <c r="K10" s="3">
+        <v>1</v>
       </c>
       <c r="L10" s="6" t="s">
         <v>19</v>
@@ -1733,29 +1768,32 @@
       <c r="M10" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="N10" s="6">
-        <v>0.03</v>
+      <c r="N10" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="O10" s="6">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="P10" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="6">
         <v>10</v>
       </c>
-      <c r="Q10" s="6" t="s">
+      <c r="R10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="R10" s="6">
+      <c r="S10" s="6">
         <v>72</v>
       </c>
-      <c r="S10" s="6">
+      <c r="T10" s="6">
         <v>70</v>
       </c>
-      <c r="T10" s="6">
+      <c r="U10" s="6">
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>39</v>
       </c>
@@ -1778,14 +1816,12 @@
       <c r="H11" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="I11" s="6"/>
+      <c r="J11" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="J11" s="3">
-        <v>1</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>19</v>
+      <c r="K11" s="3">
+        <v>1</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>19</v>
@@ -1793,29 +1829,32 @@
       <c r="M11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="N11" s="2">
-        <v>0.03</v>
+      <c r="N11" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="O11" s="2">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="P11" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="2">
         <v>35</v>
       </c>
-      <c r="Q11" s="2" t="s">
+      <c r="R11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R11" s="6">
+      <c r="S11" s="6">
         <v>18</v>
       </c>
-      <c r="S11" s="2">
+      <c r="T11" s="2">
         <v>74</v>
       </c>
-      <c r="T11" s="2">
+      <c r="U11" s="2">
         <v>82</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>39</v>
       </c>
@@ -1838,14 +1877,12 @@
       <c r="H12" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="I12" s="6" t="s">
+      <c r="I12" s="6"/>
+      <c r="J12" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="J12" s="3">
-        <v>1</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>19</v>
+      <c r="K12" s="3">
+        <v>1</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>19</v>
@@ -1853,29 +1890,32 @@
       <c r="M12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="N12" s="2">
-        <v>0.03</v>
+      <c r="N12" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="O12" s="2">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="P12" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="2">
         <v>35</v>
       </c>
-      <c r="Q12" s="2" t="s">
+      <c r="R12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R12" s="6">
+      <c r="S12" s="6">
         <v>18</v>
       </c>
-      <c r="S12" s="2">
+      <c r="T12" s="2">
         <v>74</v>
       </c>
-      <c r="T12" s="2">
+      <c r="U12" s="2">
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>39</v>
       </c>
@@ -1898,14 +1938,12 @@
       <c r="H13" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="I13" s="6" t="s">
+      <c r="I13" s="6"/>
+      <c r="J13" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="J13" s="3">
-        <v>1</v>
-      </c>
-      <c r="K13" s="6" t="s">
-        <v>19</v>
+      <c r="K13" s="3">
+        <v>1</v>
       </c>
       <c r="L13" s="6" t="s">
         <v>19</v>
@@ -1913,29 +1951,32 @@
       <c r="M13" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="N13" s="6">
-        <v>0.03</v>
+      <c r="N13" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="O13" s="6">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="P13" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="6">
         <v>35</v>
       </c>
-      <c r="Q13" s="6" t="s">
+      <c r="R13" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="R13" s="6">
+      <c r="S13" s="6">
         <v>36</v>
       </c>
-      <c r="S13" s="6">
+      <c r="T13" s="6">
         <v>74</v>
       </c>
-      <c r="T13" s="6">
+      <c r="U13" s="6">
         <v>82</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>39</v>
       </c>
@@ -1958,14 +1999,12 @@
       <c r="H14" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="I14" s="6" t="s">
+      <c r="I14" s="6"/>
+      <c r="J14" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="J14" s="3">
-        <v>1</v>
-      </c>
-      <c r="K14" s="6" t="s">
-        <v>19</v>
+      <c r="K14" s="3">
+        <v>1</v>
       </c>
       <c r="L14" s="6" t="s">
         <v>19</v>
@@ -1973,29 +2012,32 @@
       <c r="M14" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="N14" s="6">
-        <v>0.03</v>
+      <c r="N14" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="O14" s="6">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="P14" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="6">
         <v>35</v>
       </c>
-      <c r="Q14" s="6" t="s">
+      <c r="R14" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="R14" s="6">
+      <c r="S14" s="6">
         <v>36</v>
       </c>
-      <c r="S14" s="6">
+      <c r="T14" s="6">
         <v>74</v>
       </c>
-      <c r="T14" s="6">
+      <c r="U14" s="6">
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>39</v>
       </c>
@@ -2018,14 +2060,12 @@
       <c r="H15" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="I15" s="6" t="s">
+      <c r="I15" s="6"/>
+      <c r="J15" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="J15" s="3">
-        <v>1</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>19</v>
+      <c r="K15" s="3">
+        <v>1</v>
       </c>
       <c r="L15" s="2" t="s">
         <v>19</v>
@@ -2033,29 +2073,32 @@
       <c r="M15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="N15" s="2">
-        <v>0.03</v>
+      <c r="N15" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="O15" s="2">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="P15" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="2">
         <v>35</v>
       </c>
-      <c r="Q15" s="2" t="s">
+      <c r="R15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R15" s="2">
+      <c r="S15" s="2">
         <v>54</v>
       </c>
-      <c r="S15" s="2">
+      <c r="T15" s="2">
         <v>74</v>
       </c>
-      <c r="T15" s="2">
+      <c r="U15" s="2">
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>39</v>
       </c>
@@ -2078,14 +2121,12 @@
       <c r="H16" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="I16" s="6" t="s">
+      <c r="I16" s="6"/>
+      <c r="J16" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="J16" s="3">
-        <v>1</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>19</v>
+      <c r="K16" s="3">
+        <v>1</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>19</v>
@@ -2093,29 +2134,32 @@
       <c r="M16" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="N16" s="2">
-        <v>0.03</v>
+      <c r="N16" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="O16" s="2">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="P16" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="2">
         <v>35</v>
       </c>
-      <c r="Q16" s="2" t="s">
+      <c r="R16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R16" s="6">
+      <c r="S16" s="6">
         <v>54</v>
       </c>
-      <c r="S16" s="2">
+      <c r="T16" s="2">
         <v>74</v>
       </c>
-      <c r="T16" s="2">
+      <c r="U16" s="2">
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>39</v>
       </c>
@@ -2138,14 +2182,12 @@
       <c r="H17" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="I17" s="6" t="s">
+      <c r="I17" s="6"/>
+      <c r="J17" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="J17" s="3">
-        <v>1</v>
-      </c>
-      <c r="K17" s="6" t="s">
-        <v>19</v>
+      <c r="K17" s="3">
+        <v>1</v>
       </c>
       <c r="L17" s="6" t="s">
         <v>19</v>
@@ -2153,29 +2195,32 @@
       <c r="M17" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="N17" s="6">
-        <v>0.03</v>
+      <c r="N17" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="O17" s="6">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="P17" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="6">
         <v>35</v>
       </c>
-      <c r="Q17" s="6" t="s">
+      <c r="R17" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="R17" s="6">
+      <c r="S17" s="6">
         <v>72</v>
       </c>
-      <c r="S17" s="6">
+      <c r="T17" s="6">
         <v>74</v>
       </c>
-      <c r="T17" s="6">
+      <c r="U17" s="6">
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>39</v>
       </c>
@@ -2198,14 +2243,12 @@
       <c r="H18" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="I18" s="6" t="s">
+      <c r="I18" s="6"/>
+      <c r="J18" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="J18" s="3">
-        <v>1</v>
-      </c>
-      <c r="K18" s="6" t="s">
-        <v>19</v>
+      <c r="K18" s="3">
+        <v>1</v>
       </c>
       <c r="L18" s="6" t="s">
         <v>19</v>
@@ -2213,29 +2256,32 @@
       <c r="M18" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="N18" s="6">
-        <v>0.03</v>
+      <c r="N18" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="O18" s="6">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="P18" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="6">
         <v>35</v>
       </c>
-      <c r="Q18" s="6" t="s">
+      <c r="R18" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="R18" s="6">
+      <c r="S18" s="6">
         <v>72</v>
       </c>
-      <c r="S18" s="6">
+      <c r="T18" s="6">
         <v>74</v>
       </c>
-      <c r="T18" s="6">
+      <c r="U18" s="6">
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>88</v>
       </c>
@@ -2261,13 +2307,13 @@
         <v>51</v>
       </c>
       <c r="I19" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="J19" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="J19" s="3">
-        <v>1</v>
-      </c>
-      <c r="K19" s="6" t="s">
-        <v>85</v>
+      <c r="K19" s="3">
+        <v>1</v>
       </c>
       <c r="L19" s="6" t="s">
         <v>85</v>
@@ -2275,29 +2321,32 @@
       <c r="M19" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="N19" s="6">
-        <v>0.03</v>
+      <c r="N19" s="6" t="s">
+        <v>85</v>
       </c>
       <c r="O19" s="6">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="P19" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="6">
         <v>35</v>
       </c>
-      <c r="Q19" s="6" t="s">
+      <c r="R19" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="R19" s="6">
+      <c r="S19" s="6">
         <v>54</v>
       </c>
-      <c r="S19" s="6">
+      <c r="T19" s="6">
         <v>74</v>
       </c>
-      <c r="T19" s="6">
+      <c r="U19" s="6">
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>88</v>
       </c>
@@ -2323,13 +2372,13 @@
         <v>51</v>
       </c>
       <c r="I20" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="J20" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="J20" s="3">
-        <v>1</v>
-      </c>
-      <c r="K20" s="6" t="s">
-        <v>19</v>
+      <c r="K20" s="3">
+        <v>1</v>
       </c>
       <c r="L20" s="6" t="s">
         <v>19</v>
@@ -2337,29 +2386,32 @@
       <c r="M20" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="N20" s="6">
-        <v>0.03</v>
+      <c r="N20" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="O20" s="6">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="P20" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="6">
         <v>35</v>
       </c>
-      <c r="Q20" s="6" t="s">
+      <c r="R20" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="R20" s="6">
+      <c r="S20" s="6">
         <v>36</v>
       </c>
-      <c r="S20" s="6">
+      <c r="T20" s="6">
         <v>74</v>
       </c>
-      <c r="T20" s="6">
+      <c r="U20" s="6">
         <v>82</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>88</v>
       </c>
@@ -2385,13 +2437,13 @@
         <v>51</v>
       </c>
       <c r="I21" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="J21" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="J21" s="3">
-        <v>1</v>
-      </c>
-      <c r="K21" s="6" t="s">
-        <v>19</v>
+      <c r="K21" s="3">
+        <v>1</v>
       </c>
       <c r="L21" s="6" t="s">
         <v>19</v>
@@ -2399,29 +2451,32 @@
       <c r="M21" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="N21" s="6">
-        <v>0.03</v>
+      <c r="N21" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="O21" s="6">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="P21" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="6">
         <v>35</v>
       </c>
-      <c r="Q21" s="6" t="s">
+      <c r="R21" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="R21" s="6">
+      <c r="S21" s="6">
         <v>90</v>
       </c>
-      <c r="S21" s="6">
+      <c r="T21" s="6">
         <v>74</v>
       </c>
-      <c r="T21" s="6">
+      <c r="U21" s="6">
         <v>82</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>88</v>
       </c>
@@ -2447,13 +2502,13 @@
         <v>51</v>
       </c>
       <c r="I22" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="J22" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="J22" s="3">
-        <v>1</v>
-      </c>
-      <c r="K22" s="6" t="s">
-        <v>85</v>
+      <c r="K22" s="3">
+        <v>1</v>
       </c>
       <c r="L22" s="6" t="s">
         <v>85</v>
@@ -2461,29 +2516,32 @@
       <c r="M22" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="N22" s="6">
-        <v>0.03</v>
+      <c r="N22" s="6" t="s">
+        <v>85</v>
       </c>
       <c r="O22" s="6">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="P22" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="6">
         <v>35</v>
       </c>
-      <c r="Q22" s="6" t="s">
+      <c r="R22" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="R22" s="6">
+      <c r="S22" s="6">
         <v>72</v>
       </c>
-      <c r="S22" s="6">
+      <c r="T22" s="6">
         <v>74</v>
       </c>
-      <c r="T22" s="6">
+      <c r="U22" s="6">
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>120</v>
       </c>
@@ -2509,13 +2567,13 @@
         <v>111</v>
       </c>
       <c r="I23" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="J23" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="J23" s="3">
-        <v>1</v>
-      </c>
-      <c r="K23" s="6" t="s">
-        <v>85</v>
+      <c r="K23" s="3">
+        <v>1</v>
       </c>
       <c r="L23" s="6" t="s">
         <v>85</v>
@@ -2523,32 +2581,35 @@
       <c r="M23" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="N23" s="6">
-        <v>0.03</v>
+      <c r="N23" s="6" t="s">
+        <v>85</v>
       </c>
       <c r="O23" s="6">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="P23" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="6">
         <v>50</v>
       </c>
-      <c r="Q23" s="6" t="s">
+      <c r="R23" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="R23" s="6">
+      <c r="S23" s="6">
         <v>81</v>
       </c>
-      <c r="S23" s="6">
+      <c r="T23" s="6">
         <v>74</v>
       </c>
-      <c r="T23" s="6">
+      <c r="U23" s="6">
         <v>105</v>
       </c>
-      <c r="U23" s="6" t="s">
+      <c r="V23" s="6" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>120</v>
       </c>
@@ -2574,13 +2635,13 @@
         <v>111</v>
       </c>
       <c r="I24" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="J24" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="J24" s="3">
-        <v>1</v>
-      </c>
-      <c r="K24" s="6" t="s">
-        <v>19</v>
+      <c r="K24" s="3">
+        <v>1</v>
       </c>
       <c r="L24" s="6" t="s">
         <v>19</v>
@@ -2588,32 +2649,35 @@
       <c r="M24" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="N24" s="6">
-        <v>0.03</v>
+      <c r="N24" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="O24" s="6">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="P24" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q24" s="6">
         <v>50</v>
       </c>
-      <c r="Q24" s="6" t="s">
+      <c r="R24" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="R24" s="6">
+      <c r="S24" s="6">
         <v>72</v>
       </c>
-      <c r="S24" s="6">
+      <c r="T24" s="6">
         <v>74</v>
       </c>
-      <c r="T24" s="6">
+      <c r="U24" s="6">
         <v>105</v>
       </c>
-      <c r="U24" s="6" t="s">
+      <c r="V24" s="6" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>120</v>
       </c>
@@ -2639,13 +2703,13 @@
         <v>111</v>
       </c>
       <c r="I25" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="J25" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="J25" s="3">
-        <v>1</v>
-      </c>
-      <c r="K25" s="6" t="s">
-        <v>19</v>
+      <c r="K25" s="3">
+        <v>1</v>
       </c>
       <c r="L25" s="6" t="s">
         <v>19</v>
@@ -2653,32 +2717,35 @@
       <c r="M25" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="N25" s="6">
-        <v>0.03</v>
+      <c r="N25" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="O25" s="6">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="P25" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q25" s="6">
         <v>50</v>
       </c>
-      <c r="Q25" s="6" t="s">
+      <c r="R25" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="R25" s="6">
+      <c r="S25" s="6">
         <v>153</v>
       </c>
-      <c r="S25" s="6">
+      <c r="T25" s="6">
         <v>74</v>
       </c>
-      <c r="T25" s="6">
+      <c r="U25" s="6">
         <v>105</v>
       </c>
-      <c r="U25" s="6" t="s">
+      <c r="V25" s="6" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>120</v>
       </c>
@@ -2704,13 +2771,13 @@
         <v>111</v>
       </c>
       <c r="I26" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="J26" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="J26" s="3">
-        <v>1</v>
-      </c>
-      <c r="K26" s="6" t="s">
-        <v>85</v>
+      <c r="K26" s="3">
+        <v>1</v>
       </c>
       <c r="L26" s="6" t="s">
         <v>85</v>
@@ -2718,32 +2785,35 @@
       <c r="M26" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="N26" s="6">
-        <v>0.03</v>
+      <c r="N26" s="6" t="s">
+        <v>85</v>
       </c>
       <c r="O26" s="6">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="P26" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="6">
         <v>50</v>
       </c>
-      <c r="Q26" s="6" t="s">
+      <c r="R26" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="R26" s="6">
+      <c r="S26" s="6">
         <v>144</v>
       </c>
-      <c r="S26" s="6">
+      <c r="T26" s="6">
         <v>74</v>
       </c>
-      <c r="T26" s="6">
+      <c r="U26" s="6">
         <v>105</v>
       </c>
-      <c r="U26" s="6" t="s">
+      <c r="V26" s="6" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>40</v>
       </c>
@@ -2766,14 +2836,12 @@
       <c r="H27" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="I27" s="6" t="s">
+      <c r="I27" s="6"/>
+      <c r="J27" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="J27" s="3">
-        <v>1</v>
-      </c>
-      <c r="K27" s="2" t="s">
-        <v>19</v>
+      <c r="K27" s="3">
+        <v>1</v>
       </c>
       <c r="L27" s="2" t="s">
         <v>19</v>
@@ -2781,32 +2849,35 @@
       <c r="M27" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="N27" s="2">
-        <v>0.03</v>
+      <c r="N27" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="O27" s="2">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="P27" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q27" s="2">
         <v>50</v>
       </c>
-      <c r="Q27" s="2" t="s">
+      <c r="R27" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R27" s="6">
+      <c r="S27" s="6">
         <v>27</v>
       </c>
-      <c r="S27" s="2">
+      <c r="T27" s="2">
         <v>74</v>
       </c>
-      <c r="T27" s="2">
+      <c r="U27" s="2">
         <v>82</v>
       </c>
-      <c r="U27" s="6" t="s">
+      <c r="V27" s="6" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>40</v>
       </c>
@@ -2829,14 +2900,12 @@
       <c r="H28" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="I28" s="6" t="s">
+      <c r="I28" s="6"/>
+      <c r="J28" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="J28" s="3">
-        <v>1</v>
-      </c>
-      <c r="K28" s="6" t="s">
-        <v>19</v>
+      <c r="K28" s="3">
+        <v>1</v>
       </c>
       <c r="L28" s="6" t="s">
         <v>19</v>
@@ -2844,32 +2913,35 @@
       <c r="M28" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="N28" s="6">
-        <v>0.03</v>
+      <c r="N28" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="O28" s="6">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="P28" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="6">
         <v>50</v>
       </c>
-      <c r="Q28" s="6" t="s">
+      <c r="R28" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="R28" s="6">
+      <c r="S28" s="6">
         <v>54</v>
       </c>
-      <c r="S28" s="6">
+      <c r="T28" s="6">
         <v>74</v>
       </c>
-      <c r="T28" s="6">
+      <c r="U28" s="6">
         <v>82</v>
       </c>
-      <c r="U28" s="6" t="s">
+      <c r="V28" s="6" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>40</v>
       </c>
@@ -2892,14 +2964,12 @@
       <c r="H29" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="I29" s="6" t="s">
+      <c r="I29" s="6"/>
+      <c r="J29" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="J29" s="3">
-        <v>1</v>
-      </c>
-      <c r="K29" s="2" t="s">
-        <v>19</v>
+      <c r="K29" s="3">
+        <v>1</v>
       </c>
       <c r="L29" s="2" t="s">
         <v>19</v>
@@ -2907,32 +2977,35 @@
       <c r="M29" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="N29" s="2">
-        <v>0.03</v>
+      <c r="N29" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="O29" s="2">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="P29" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q29" s="2">
         <v>50</v>
       </c>
-      <c r="Q29" s="2" t="s">
+      <c r="R29" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R29" s="6">
+      <c r="S29" s="6">
         <v>27</v>
       </c>
-      <c r="S29" s="2">
+      <c r="T29" s="2">
         <v>74</v>
       </c>
-      <c r="T29" s="2">
+      <c r="U29" s="2">
         <v>82</v>
       </c>
-      <c r="U29" s="6" t="s">
+      <c r="V29" s="6" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>40</v>
       </c>
@@ -2955,14 +3028,12 @@
       <c r="H30" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="I30" s="6" t="s">
+      <c r="I30" s="6"/>
+      <c r="J30" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="J30" s="3">
-        <v>1</v>
-      </c>
-      <c r="K30" s="6" t="s">
-        <v>19</v>
+      <c r="K30" s="3">
+        <v>1</v>
       </c>
       <c r="L30" s="6" t="s">
         <v>19</v>
@@ -2970,32 +3041,35 @@
       <c r="M30" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="N30" s="6">
-        <v>0.03</v>
+      <c r="N30" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="O30" s="6">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="P30" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q30" s="6">
         <v>50</v>
       </c>
-      <c r="Q30" s="6" t="s">
+      <c r="R30" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="R30" s="6">
+      <c r="S30" s="6">
         <v>54</v>
       </c>
-      <c r="S30" s="6">
+      <c r="T30" s="6">
         <v>74</v>
       </c>
-      <c r="T30" s="6">
+      <c r="U30" s="6">
         <v>82</v>
       </c>
-      <c r="U30" s="6" t="s">
+      <c r="V30" s="6" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>40</v>
       </c>
@@ -3017,14 +3091,12 @@
       <c r="H31" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="I31" s="6" t="s">
+      <c r="I31" s="6"/>
+      <c r="J31" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="J31" s="3">
-        <v>1</v>
-      </c>
-      <c r="K31" s="2" t="s">
-        <v>19</v>
+      <c r="K31" s="3">
+        <v>1</v>
       </c>
       <c r="L31" s="2" t="s">
         <v>19</v>
@@ -3032,32 +3104,35 @@
       <c r="M31" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="N31" s="2">
-        <v>0.03</v>
+      <c r="N31" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="O31" s="2">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="P31" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q31" s="2">
         <v>50</v>
       </c>
-      <c r="Q31" s="2" t="s">
+      <c r="R31" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R31" s="6">
+      <c r="S31" s="6">
         <v>81</v>
       </c>
-      <c r="S31" s="2">
+      <c r="T31" s="2">
         <v>74</v>
       </c>
-      <c r="T31" s="2">
+      <c r="U31" s="2">
         <v>82</v>
       </c>
-      <c r="U31" s="6" t="s">
+      <c r="V31" s="6" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>40</v>
       </c>
@@ -3079,14 +3154,12 @@
       <c r="H32" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="I32" s="6" t="s">
+      <c r="I32" s="6"/>
+      <c r="J32" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="J32" s="3">
-        <v>1</v>
-      </c>
-      <c r="K32" s="6" t="s">
-        <v>19</v>
+      <c r="K32" s="3">
+        <v>1</v>
       </c>
       <c r="L32" s="6" t="s">
         <v>19</v>
@@ -3094,32 +3167,35 @@
       <c r="M32" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="N32" s="6">
-        <v>0.03</v>
+      <c r="N32" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="O32" s="6">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="P32" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q32" s="6">
         <v>50</v>
       </c>
-      <c r="Q32" s="6" t="s">
+      <c r="R32" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="R32" s="6">
+      <c r="S32" s="6">
         <v>108</v>
       </c>
-      <c r="S32" s="6">
+      <c r="T32" s="6">
         <v>74</v>
       </c>
-      <c r="T32" s="6">
+      <c r="U32" s="6">
         <v>82</v>
       </c>
-      <c r="U32" s="6" t="s">
+      <c r="V32" s="6" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>40</v>
       </c>
@@ -3141,14 +3217,12 @@
       <c r="H33" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="I33" s="6" t="s">
+      <c r="I33" s="6"/>
+      <c r="J33" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="J33" s="3">
-        <v>1</v>
-      </c>
-      <c r="K33" s="2" t="s">
-        <v>19</v>
+      <c r="K33" s="3">
+        <v>1</v>
       </c>
       <c r="L33" s="2" t="s">
         <v>19</v>
@@ -3156,32 +3230,35 @@
       <c r="M33" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="N33" s="2">
-        <v>0.03</v>
+      <c r="N33" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="O33" s="2">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="P33" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q33" s="2">
         <v>50</v>
       </c>
-      <c r="Q33" s="2" t="s">
+      <c r="R33" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R33" s="6">
+      <c r="S33" s="6">
         <v>81</v>
       </c>
-      <c r="S33" s="2">
+      <c r="T33" s="2">
         <v>74</v>
       </c>
-      <c r="T33" s="2">
+      <c r="U33" s="2">
         <v>82</v>
       </c>
-      <c r="U33" s="6" t="s">
+      <c r="V33" s="6" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>40</v>
       </c>
@@ -3203,14 +3280,12 @@
       <c r="H34" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="I34" s="6" t="s">
+      <c r="I34" s="6"/>
+      <c r="J34" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="J34" s="3">
-        <v>1</v>
-      </c>
-      <c r="K34" s="6" t="s">
-        <v>19</v>
+      <c r="K34" s="3">
+        <v>1</v>
       </c>
       <c r="L34" s="6" t="s">
         <v>19</v>
@@ -3218,66 +3293,69 @@
       <c r="M34" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="N34" s="6">
-        <v>0.03</v>
+      <c r="N34" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="O34" s="6">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="P34" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q34" s="6">
         <v>50</v>
       </c>
-      <c r="Q34" s="6" t="s">
+      <c r="R34" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="R34" s="6">
+      <c r="S34" s="6">
         <v>108</v>
       </c>
-      <c r="S34" s="6">
+      <c r="T34" s="6">
         <v>74</v>
       </c>
-      <c r="T34" s="6">
+      <c r="U34" s="6">
         <v>82</v>
       </c>
-      <c r="U34" s="6" t="s">
+      <c r="V34" s="6" t="s">
         <v>179</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:T2"/>
+  <autoFilter ref="A2:U2"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U35"/>
+  <dimension ref="A1:V35"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.625" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.625" customWidth="1"/>
-    <col min="7" max="7" width="16.25" customWidth="1"/>
-    <col min="8" max="8" width="8.625" customWidth="1"/>
-    <col min="9" max="9" width="18.125" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5" hidden="1" customWidth="1"/>
-    <col min="11" max="13" width="0" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="10.625" hidden="1" customWidth="1"/>
-    <col min="15" max="16" width="8.625" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="13.5" hidden="1" customWidth="1"/>
-    <col min="18" max="20" width="8.625" customWidth="1"/>
+    <col min="5" max="5" width="30.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" customWidth="1"/>
+    <col min="7" max="7" width="16.21875" customWidth="1"/>
+    <col min="8" max="9" width="8.6640625" customWidth="1"/>
+    <col min="10" max="10" width="18.109375" customWidth="1"/>
+    <col min="11" max="11" width="12.44140625" customWidth="1"/>
+    <col min="12" max="14" width="8.88671875" customWidth="1"/>
+    <col min="15" max="15" width="10.6640625" customWidth="1"/>
+    <col min="16" max="17" width="8.6640625" customWidth="1"/>
+    <col min="18" max="18" width="13.44140625" customWidth="1"/>
+    <col min="19" max="21" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" s="1" customFormat="1" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3303,46 +3381,49 @@
         <v>17</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="1" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" s="1" customFormat="1" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>33</v>
       </c>
@@ -3368,46 +3449,49 @@
         <v>16</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Q2" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="R2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>81</v>
       </c>
@@ -3428,42 +3512,43 @@
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="6"/>
+      <c r="J3" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="L3" s="2" t="s">
         <v>19</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="N3" s="2">
-        <v>0.03</v>
+      <c r="N3" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="O3" s="2">
-        <v>1</v>
-      </c>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2" t="s">
+        <v>0.03</v>
+      </c>
+      <c r="P3" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="R3" s="2">
+      <c r="S3" s="2">
         <v>105</v>
       </c>
-      <c r="S3" s="2">
+      <c r="T3" s="2">
         <v>86</v>
       </c>
-      <c r="T3" s="2">
+      <c r="U3" s="2">
         <v>161</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>44</v>
       </c>
@@ -3484,42 +3569,43 @@
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="6"/>
+      <c r="J4" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K4" s="6" t="s">
-        <v>19</v>
-      </c>
       <c r="L4" s="6" t="s">
         <v>19</v>
       </c>
       <c r="M4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="N4" s="6">
-        <v>0.03</v>
+      <c r="N4" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="O4" s="6">
-        <v>1</v>
-      </c>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6" t="s">
+        <v>0.03</v>
+      </c>
+      <c r="P4" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="R4" s="6">
+      <c r="S4" s="6">
         <v>105</v>
       </c>
-      <c r="S4" s="6">
+      <c r="T4" s="6">
         <v>86</v>
       </c>
-      <c r="T4" s="6">
+      <c r="U4" s="6">
         <v>161</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>44</v>
       </c>
@@ -3540,42 +3626,43 @@
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="6"/>
+      <c r="J5" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="K5" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K5" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="L5" s="2" t="s">
         <v>19</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="N5" s="2">
-        <v>0.03</v>
+      <c r="N5" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="O5" s="2">
-        <v>1</v>
-      </c>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2" t="s">
+        <v>0.03</v>
+      </c>
+      <c r="P5" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="R5" s="6">
+      <c r="S5" s="6">
         <v>105</v>
       </c>
-      <c r="S5" s="2">
+      <c r="T5" s="2">
         <v>86</v>
       </c>
-      <c r="T5" s="2">
+      <c r="U5" s="2">
         <v>161</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>164</v>
       </c>
@@ -3598,42 +3685,45 @@
         <v>170</v>
       </c>
       <c r="H6" s="6"/>
-      <c r="I6" s="4" t="s">
+      <c r="I6" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="J6" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="K6" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K6" s="6" t="s">
-        <v>19</v>
-      </c>
       <c r="L6" s="6" t="s">
         <v>19</v>
       </c>
       <c r="M6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="N6" s="6">
-        <v>0.03</v>
+      <c r="N6" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="O6" s="6">
-        <v>1</v>
-      </c>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="6" t="s">
+        <v>0.03</v>
+      </c>
+      <c r="P6" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="R6" s="6">
+      <c r="S6" s="6">
         <v>105</v>
       </c>
-      <c r="S6" s="6">
+      <c r="T6" s="6">
         <v>86</v>
       </c>
-      <c r="T6" s="6">
+      <c r="U6" s="6">
         <v>161</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>44</v>
       </c>
@@ -3654,42 +3744,42 @@
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
-      <c r="I7" s="4" t="s">
+      <c r="J7" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="K7" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K7" s="6" t="s">
-        <v>19</v>
-      </c>
       <c r="L7" s="6" t="s">
         <v>19</v>
       </c>
       <c r="M7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="N7" s="6">
-        <v>0.03</v>
+      <c r="N7" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="O7" s="6">
-        <v>1</v>
-      </c>
-      <c r="P7" s="6"/>
-      <c r="Q7" s="6" t="s">
+        <v>0.03</v>
+      </c>
+      <c r="P7" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="R7" s="6">
+      <c r="S7" s="6">
         <v>140</v>
       </c>
-      <c r="S7" s="6">
+      <c r="T7" s="6">
         <v>86</v>
       </c>
-      <c r="T7" s="6">
+      <c r="U7" s="6">
         <v>161</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>44</v>
       </c>
@@ -3710,42 +3800,42 @@
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
-      <c r="I8" s="4" t="s">
+      <c r="J8" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="K8" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K8" s="6" t="s">
-        <v>19</v>
-      </c>
       <c r="L8" s="6" t="s">
         <v>19</v>
       </c>
       <c r="M8" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="N8" s="6">
-        <v>0.03</v>
+      <c r="N8" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="O8" s="6">
-        <v>1</v>
-      </c>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="6" t="s">
+        <v>0.03</v>
+      </c>
+      <c r="P8" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="R8" s="6">
+      <c r="S8" s="6">
         <v>140</v>
       </c>
-      <c r="S8" s="6">
+      <c r="T8" s="6">
         <v>86</v>
       </c>
-      <c r="T8" s="6">
+      <c r="U8" s="6">
         <v>161</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>44</v>
       </c>
@@ -3766,42 +3856,42 @@
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="4" t="s">
+      <c r="J9" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="J9" s="3" t="s">
+      <c r="K9" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K9" s="6" t="s">
-        <v>19</v>
-      </c>
       <c r="L9" s="6" t="s">
         <v>19</v>
       </c>
       <c r="M9" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="N9" s="6">
-        <v>0.03</v>
+      <c r="N9" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="O9" s="6">
-        <v>1</v>
-      </c>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="6" t="s">
+        <v>0.03</v>
+      </c>
+      <c r="P9" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="R9" s="6">
+      <c r="S9" s="6">
         <v>140</v>
       </c>
-      <c r="S9" s="6">
+      <c r="T9" s="6">
         <v>86</v>
       </c>
-      <c r="T9" s="6">
+      <c r="U9" s="6">
         <v>161</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>164</v>
       </c>
@@ -3824,42 +3914,45 @@
         <v>170</v>
       </c>
       <c r="H10" s="6"/>
-      <c r="I10" s="4" t="s">
+      <c r="I10" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="J10" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="J10" s="3" t="s">
+      <c r="K10" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K10" s="6" t="s">
-        <v>19</v>
-      </c>
       <c r="L10" s="6" t="s">
         <v>19</v>
       </c>
       <c r="M10" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="N10" s="6">
-        <v>0.03</v>
+      <c r="N10" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="O10" s="6">
-        <v>1</v>
-      </c>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="6" t="s">
+        <v>0.03</v>
+      </c>
+      <c r="P10" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="R10" s="6">
+      <c r="S10" s="6">
         <v>140</v>
       </c>
-      <c r="S10" s="6">
+      <c r="T10" s="6">
         <v>86</v>
       </c>
-      <c r="T10" s="6">
+      <c r="U10" s="6">
         <v>161</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>48</v>
       </c>
@@ -3880,42 +3973,43 @@
       </c>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
-      <c r="I11" s="4" t="s">
+      <c r="I11" s="6"/>
+      <c r="J11" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="J11" s="3" t="s">
+      <c r="K11" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K11" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="L11" s="2" t="s">
         <v>19</v>
       </c>
       <c r="M11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="N11" s="2">
-        <v>0.03</v>
+      <c r="N11" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="O11" s="2">
-        <v>1</v>
-      </c>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2" t="s">
+        <v>0.03</v>
+      </c>
+      <c r="P11" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="R11" s="6">
+      <c r="S11" s="6">
         <v>105</v>
       </c>
-      <c r="S11" s="2">
+      <c r="T11" s="2">
         <v>86</v>
       </c>
-      <c r="T11" s="2">
+      <c r="U11" s="2">
         <v>161</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>48</v>
       </c>
@@ -3936,42 +4030,43 @@
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
-      <c r="I12" s="4" t="s">
+      <c r="I12" s="6"/>
+      <c r="J12" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="J12" s="3" t="s">
+      <c r="K12" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K12" s="6" t="s">
-        <v>19</v>
-      </c>
       <c r="L12" s="6" t="s">
         <v>19</v>
       </c>
       <c r="M12" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="N12" s="6">
-        <v>0.03</v>
+      <c r="N12" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="O12" s="6">
-        <v>1</v>
-      </c>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6" t="s">
+        <v>0.03</v>
+      </c>
+      <c r="P12" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="R12" s="6">
+      <c r="S12" s="6">
         <v>105</v>
       </c>
-      <c r="S12" s="6">
+      <c r="T12" s="6">
         <v>86</v>
       </c>
-      <c r="T12" s="6">
+      <c r="U12" s="6">
         <v>161</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>48</v>
       </c>
@@ -3992,42 +4087,43 @@
       </c>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
-      <c r="I13" s="4" t="s">
+      <c r="I13" s="6"/>
+      <c r="J13" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="J13" s="3" t="s">
+      <c r="K13" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K13" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="L13" s="2" t="s">
         <v>19</v>
       </c>
       <c r="M13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="N13" s="2">
-        <v>0.03</v>
+      <c r="N13" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="O13" s="2">
-        <v>1</v>
-      </c>
-      <c r="P13" s="2"/>
-      <c r="Q13" s="2" t="s">
+        <v>0.03</v>
+      </c>
+      <c r="P13" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="R13" s="6">
+      <c r="S13" s="6">
         <v>105</v>
       </c>
-      <c r="S13" s="2">
+      <c r="T13" s="2">
         <v>86</v>
       </c>
-      <c r="T13" s="2">
+      <c r="U13" s="2">
         <v>161</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>171</v>
       </c>
@@ -4050,42 +4146,45 @@
         <v>170</v>
       </c>
       <c r="H14" s="6"/>
-      <c r="I14" s="4" t="s">
+      <c r="I14" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="J14" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="J14" s="3" t="s">
+      <c r="K14" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K14" s="6" t="s">
-        <v>19</v>
-      </c>
       <c r="L14" s="6" t="s">
         <v>19</v>
       </c>
       <c r="M14" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="N14" s="6">
-        <v>0.03</v>
+      <c r="N14" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="O14" s="6">
-        <v>1</v>
-      </c>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="6" t="s">
+        <v>0.03</v>
+      </c>
+      <c r="P14" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="R14" s="6">
+      <c r="S14" s="6">
         <v>105</v>
       </c>
-      <c r="S14" s="6">
+      <c r="T14" s="6">
         <v>86</v>
       </c>
-      <c r="T14" s="6">
+      <c r="U14" s="6">
         <v>161</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>48</v>
       </c>
@@ -4106,42 +4205,43 @@
       </c>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
-      <c r="I15" s="4" t="s">
+      <c r="I15" s="6"/>
+      <c r="J15" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="J15" s="3" t="s">
+      <c r="K15" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K15" s="6" t="s">
-        <v>19</v>
-      </c>
       <c r="L15" s="6" t="s">
         <v>19</v>
       </c>
       <c r="M15" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="N15" s="6">
-        <v>0.03</v>
+      <c r="N15" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="O15" s="6">
-        <v>1</v>
-      </c>
-      <c r="P15" s="6"/>
-      <c r="Q15" s="6" t="s">
+        <v>0.03</v>
+      </c>
+      <c r="P15" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="R15" s="6">
+      <c r="S15" s="6">
         <v>140</v>
       </c>
-      <c r="S15" s="6">
+      <c r="T15" s="6">
         <v>86</v>
       </c>
-      <c r="T15" s="6">
+      <c r="U15" s="6">
         <v>161</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>48</v>
       </c>
@@ -4162,42 +4262,43 @@
       </c>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
-      <c r="I16" s="4" t="s">
+      <c r="I16" s="6"/>
+      <c r="J16" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="J16" s="3" t="s">
+      <c r="K16" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K16" s="6" t="s">
-        <v>19</v>
-      </c>
       <c r="L16" s="6" t="s">
         <v>19</v>
       </c>
       <c r="M16" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="N16" s="6">
-        <v>0.03</v>
+      <c r="N16" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="O16" s="6">
-        <v>1</v>
-      </c>
-      <c r="P16" s="6"/>
-      <c r="Q16" s="6" t="s">
+        <v>0.03</v>
+      </c>
+      <c r="P16" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="R16" s="6">
+      <c r="S16" s="6">
         <v>140</v>
       </c>
-      <c r="S16" s="6">
+      <c r="T16" s="6">
         <v>86</v>
       </c>
-      <c r="T16" s="6">
+      <c r="U16" s="6">
         <v>161</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>48</v>
       </c>
@@ -4218,42 +4319,43 @@
       </c>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
-      <c r="I17" s="4" t="s">
+      <c r="I17" s="6"/>
+      <c r="J17" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="J17" s="3" t="s">
+      <c r="K17" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K17" s="6" t="s">
-        <v>19</v>
-      </c>
       <c r="L17" s="6" t="s">
         <v>19</v>
       </c>
       <c r="M17" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="N17" s="6">
-        <v>0.03</v>
+      <c r="N17" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="O17" s="6">
-        <v>1</v>
-      </c>
-      <c r="P17" s="6"/>
-      <c r="Q17" s="6" t="s">
+        <v>0.03</v>
+      </c>
+      <c r="P17" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="R17" s="6">
+      <c r="S17" s="6">
         <v>140</v>
       </c>
-      <c r="S17" s="6">
+      <c r="T17" s="6">
         <v>86</v>
       </c>
-      <c r="T17" s="6">
+      <c r="U17" s="6">
         <v>161</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>172</v>
       </c>
@@ -4276,42 +4378,45 @@
         <v>170</v>
       </c>
       <c r="H18" s="6"/>
-      <c r="I18" s="4" t="s">
+      <c r="I18" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="J18" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="J18" s="3" t="s">
+      <c r="K18" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K18" s="6" t="s">
-        <v>19</v>
-      </c>
       <c r="L18" s="6" t="s">
         <v>19</v>
       </c>
       <c r="M18" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="N18" s="6">
-        <v>0.03</v>
+      <c r="N18" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="O18" s="6">
-        <v>1</v>
-      </c>
-      <c r="P18" s="6"/>
-      <c r="Q18" s="6" t="s">
+        <v>0.03</v>
+      </c>
+      <c r="P18" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="R18" s="6">
+      <c r="S18" s="6">
         <v>140</v>
       </c>
-      <c r="S18" s="6">
+      <c r="T18" s="6">
         <v>86</v>
       </c>
-      <c r="T18" s="6">
+      <c r="U18" s="6">
         <v>161</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>56</v>
       </c>
@@ -4331,42 +4436,42 @@
         <v>80</v>
       </c>
       <c r="G19" s="6"/>
-      <c r="I19" s="4" t="s">
+      <c r="J19" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="J19" s="3" t="s">
+      <c r="K19" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K19" s="6" t="s">
-        <v>19</v>
-      </c>
       <c r="L19" s="6" t="s">
         <v>19</v>
       </c>
       <c r="M19" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="N19" s="6">
-        <v>0.03</v>
+      <c r="N19" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="O19" s="6">
-        <v>1</v>
-      </c>
-      <c r="P19" s="6"/>
-      <c r="Q19" s="6" t="s">
+        <v>0.03</v>
+      </c>
+      <c r="P19" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="R19" s="6">
+      <c r="S19" s="6">
         <v>105</v>
       </c>
-      <c r="S19" s="6">
+      <c r="T19" s="6">
         <v>86</v>
       </c>
-      <c r="T19" s="6">
+      <c r="U19" s="6">
         <v>161</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>56</v>
       </c>
@@ -4386,42 +4491,42 @@
         <v>79</v>
       </c>
       <c r="G20" s="6"/>
-      <c r="I20" s="4" t="s">
+      <c r="J20" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="J20" s="3" t="s">
+      <c r="K20" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K20" s="6" t="s">
-        <v>19</v>
-      </c>
       <c r="L20" s="6" t="s">
         <v>19</v>
       </c>
       <c r="M20" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="N20" s="6">
-        <v>0.03</v>
+      <c r="N20" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="O20" s="6">
-        <v>1</v>
-      </c>
-      <c r="P20" s="6"/>
-      <c r="Q20" s="6" t="s">
+        <v>0.03</v>
+      </c>
+      <c r="P20" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="R20" s="6">
+      <c r="S20" s="6">
         <v>105</v>
       </c>
-      <c r="S20" s="6">
+      <c r="T20" s="6">
         <v>86</v>
       </c>
-      <c r="T20" s="6">
+      <c r="U20" s="6">
         <v>161</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>56</v>
       </c>
@@ -4441,42 +4546,42 @@
         <v>42</v>
       </c>
       <c r="G21" s="6"/>
-      <c r="I21" s="4" t="s">
+      <c r="J21" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="J21" s="3" t="s">
+      <c r="K21" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K21" s="6" t="s">
-        <v>19</v>
-      </c>
       <c r="L21" s="6" t="s">
         <v>19</v>
       </c>
       <c r="M21" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="N21" s="6">
-        <v>0.03</v>
+      <c r="N21" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="O21" s="6">
-        <v>1</v>
-      </c>
-      <c r="P21" s="6"/>
-      <c r="Q21" s="6" t="s">
+        <v>0.03</v>
+      </c>
+      <c r="P21" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="R21" s="6">
+      <c r="S21" s="6">
         <v>105</v>
       </c>
-      <c r="S21" s="6">
+      <c r="T21" s="6">
         <v>86</v>
       </c>
-      <c r="T21" s="6">
+      <c r="U21" s="6">
         <v>161</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>173</v>
       </c>
@@ -4498,42 +4603,45 @@
       <c r="G22" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="I22" s="4" t="s">
+      <c r="I22" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="J22" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="3" t="s">
+      <c r="K22" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K22" s="6" t="s">
-        <v>19</v>
-      </c>
       <c r="L22" s="6" t="s">
         <v>19</v>
       </c>
       <c r="M22" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="N22" s="6">
-        <v>0.03</v>
+      <c r="N22" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="O22" s="6">
-        <v>1</v>
-      </c>
-      <c r="P22" s="6"/>
-      <c r="Q22" s="6" t="s">
+        <v>0.03</v>
+      </c>
+      <c r="P22" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="6"/>
+      <c r="R22" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="R22" s="6">
+      <c r="S22" s="6">
         <v>105</v>
       </c>
-      <c r="S22" s="6">
+      <c r="T22" s="6">
         <v>86</v>
       </c>
-      <c r="T22" s="6">
+      <c r="U22" s="6">
         <v>161</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>56</v>
       </c>
@@ -4553,42 +4661,43 @@
         <v>79</v>
       </c>
       <c r="G23" s="6"/>
-      <c r="I23" s="4" t="s">
+      <c r="I23" s="6"/>
+      <c r="J23" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="3" t="s">
+      <c r="K23" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K23" s="6" t="s">
-        <v>19</v>
-      </c>
       <c r="L23" s="6" t="s">
         <v>19</v>
       </c>
       <c r="M23" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="N23" s="6">
-        <v>0.03</v>
+      <c r="N23" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="O23" s="6">
-        <v>1</v>
-      </c>
-      <c r="P23" s="6"/>
-      <c r="Q23" s="6" t="s">
+        <v>0.03</v>
+      </c>
+      <c r="P23" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="6"/>
+      <c r="R23" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="R23" s="6">
+      <c r="S23" s="6">
         <v>140</v>
       </c>
-      <c r="S23" s="6">
+      <c r="T23" s="6">
         <v>86</v>
       </c>
-      <c r="T23" s="6">
+      <c r="U23" s="6">
         <v>161</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>56</v>
       </c>
@@ -4608,42 +4717,43 @@
         <v>79</v>
       </c>
       <c r="G24" s="6"/>
-      <c r="I24" s="4" t="s">
+      <c r="I24" s="6"/>
+      <c r="J24" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="J24" s="3" t="s">
+      <c r="K24" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K24" s="6" t="s">
-        <v>19</v>
-      </c>
       <c r="L24" s="6" t="s">
         <v>19</v>
       </c>
       <c r="M24" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="N24" s="6">
-        <v>0.03</v>
+      <c r="N24" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="O24" s="6">
-        <v>1</v>
-      </c>
-      <c r="P24" s="6"/>
-      <c r="Q24" s="6" t="s">
+        <v>0.03</v>
+      </c>
+      <c r="P24" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q24" s="6"/>
+      <c r="R24" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="R24" s="6">
+      <c r="S24" s="6">
         <v>140</v>
       </c>
-      <c r="S24" s="6">
+      <c r="T24" s="6">
         <v>86</v>
       </c>
-      <c r="T24" s="6">
+      <c r="U24" s="6">
         <v>161</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>56</v>
       </c>
@@ -4663,42 +4773,43 @@
         <v>42</v>
       </c>
       <c r="G25" s="6"/>
-      <c r="I25" s="4" t="s">
+      <c r="I25" s="6"/>
+      <c r="J25" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="J25" s="3" t="s">
+      <c r="K25" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K25" s="6" t="s">
-        <v>19</v>
-      </c>
       <c r="L25" s="6" t="s">
         <v>19</v>
       </c>
       <c r="M25" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="N25" s="6">
-        <v>0.03</v>
+      <c r="N25" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="O25" s="6">
-        <v>1</v>
-      </c>
-      <c r="P25" s="6"/>
-      <c r="Q25" s="6" t="s">
+        <v>0.03</v>
+      </c>
+      <c r="P25" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q25" s="6"/>
+      <c r="R25" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="R25" s="6">
+      <c r="S25" s="6">
         <v>140</v>
       </c>
-      <c r="S25" s="6">
+      <c r="T25" s="6">
         <v>86</v>
       </c>
-      <c r="T25" s="6">
+      <c r="U25" s="6">
         <v>161</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>174</v>
       </c>
@@ -4720,42 +4831,45 @@
       <c r="G26" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="I26" s="4" t="s">
+      <c r="I26" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="J26" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="J26" s="3" t="s">
+      <c r="K26" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K26" s="6" t="s">
-        <v>19</v>
-      </c>
       <c r="L26" s="6" t="s">
         <v>19</v>
       </c>
       <c r="M26" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="N26" s="6">
-        <v>0.03</v>
+      <c r="N26" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="O26" s="6">
-        <v>1</v>
-      </c>
-      <c r="P26" s="6"/>
-      <c r="Q26" s="6" t="s">
+        <v>0.03</v>
+      </c>
+      <c r="P26" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="6"/>
+      <c r="R26" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="R26" s="6">
+      <c r="S26" s="6">
         <v>140</v>
       </c>
-      <c r="S26" s="6">
+      <c r="T26" s="6">
         <v>86</v>
       </c>
-      <c r="T26" s="6">
+      <c r="U26" s="6">
         <v>161</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>59</v>
       </c>
@@ -4775,42 +4889,43 @@
         <v>42</v>
       </c>
       <c r="G27" s="6"/>
-      <c r="I27" s="4" t="s">
+      <c r="I27" s="6"/>
+      <c r="J27" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="J27" s="3" t="s">
+      <c r="K27" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K27" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="L27" s="6">
+      <c r="L27" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M27" s="6">
         <v>5</v>
       </c>
-      <c r="M27" s="6">
-        <v>1</v>
-      </c>
       <c r="N27" s="6">
-        <v>0.03</v>
+        <v>1</v>
       </c>
       <c r="O27" s="6">
-        <v>1</v>
-      </c>
-      <c r="P27" s="6"/>
-      <c r="Q27" s="6" t="s">
+        <v>0.03</v>
+      </c>
+      <c r="P27" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q27" s="6"/>
+      <c r="R27" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="R27" s="6">
+      <c r="S27" s="6">
         <v>140</v>
       </c>
-      <c r="S27" s="6">
+      <c r="T27" s="6">
         <v>110</v>
       </c>
-      <c r="T27" s="6">
+      <c r="U27" s="6">
         <v>255</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>175</v>
       </c>
@@ -4832,42 +4947,45 @@
       <c r="G28" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="I28" s="4" t="s">
+      <c r="I28" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="J28" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="J28" s="3" t="s">
+      <c r="K28" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K28" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="L28" s="6">
+      <c r="L28" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M28" s="6">
         <v>5</v>
       </c>
-      <c r="M28" s="6">
-        <v>1</v>
-      </c>
       <c r="N28" s="6">
-        <v>0.03</v>
+        <v>1</v>
       </c>
       <c r="O28" s="6">
-        <v>1</v>
-      </c>
-      <c r="P28" s="6"/>
-      <c r="Q28" s="6" t="s">
+        <v>0.03</v>
+      </c>
+      <c r="P28" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="6"/>
+      <c r="R28" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="R28" s="6">
+      <c r="S28" s="6">
         <v>140</v>
       </c>
-      <c r="S28" s="6">
+      <c r="T28" s="6">
         <v>110</v>
       </c>
-      <c r="T28" s="6">
+      <c r="U28" s="6">
         <v>255</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>59</v>
       </c>
@@ -4887,42 +5005,43 @@
         <v>42</v>
       </c>
       <c r="G29" s="6"/>
-      <c r="I29" s="4" t="s">
+      <c r="I29" s="6"/>
+      <c r="J29" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="J29" s="3" t="s">
+      <c r="K29" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K29" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="L29" s="6">
+      <c r="L29" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M29" s="6">
         <v>5</v>
       </c>
-      <c r="M29" s="6">
-        <v>1</v>
-      </c>
       <c r="N29" s="6">
-        <v>0.03</v>
+        <v>1</v>
       </c>
       <c r="O29" s="6">
-        <v>1</v>
-      </c>
-      <c r="P29" s="6"/>
-      <c r="Q29" s="6" t="s">
+        <v>0.03</v>
+      </c>
+      <c r="P29" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q29" s="6"/>
+      <c r="R29" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="R29" s="6">
+      <c r="S29" s="6">
         <v>185</v>
       </c>
-      <c r="S29" s="6">
+      <c r="T29" s="6">
         <v>110</v>
       </c>
-      <c r="T29" s="6">
+      <c r="U29" s="6">
         <v>255</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>176</v>
       </c>
@@ -4944,42 +5063,45 @@
       <c r="G30" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="I30" s="4" t="s">
+      <c r="I30" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="J30" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="J30" s="3" t="s">
+      <c r="K30" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K30" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="L30" s="6">
+      <c r="L30" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M30" s="6">
         <v>5</v>
       </c>
-      <c r="M30" s="6">
-        <v>1</v>
-      </c>
       <c r="N30" s="6">
-        <v>0.03</v>
+        <v>1</v>
       </c>
       <c r="O30" s="6">
-        <v>1</v>
-      </c>
-      <c r="P30" s="6"/>
-      <c r="Q30" s="6" t="s">
+        <v>0.03</v>
+      </c>
+      <c r="P30" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q30" s="6"/>
+      <c r="R30" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="R30" s="6">
+      <c r="S30" s="6">
         <v>185</v>
       </c>
-      <c r="S30" s="6">
+      <c r="T30" s="6">
         <v>110</v>
       </c>
-      <c r="T30" s="6">
+      <c r="U30" s="6">
         <v>255</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>65</v>
       </c>
@@ -4999,42 +5121,43 @@
         <v>42</v>
       </c>
       <c r="G31" s="6"/>
-      <c r="I31" s="4" t="s">
+      <c r="I31" s="6"/>
+      <c r="J31" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="J31" s="3" t="s">
+      <c r="K31" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K31" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="L31" s="6">
+      <c r="L31" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M31" s="6">
         <v>6</v>
       </c>
-      <c r="M31" s="6">
-        <v>1</v>
-      </c>
       <c r="N31" s="6">
-        <v>0.03</v>
+        <v>1</v>
       </c>
       <c r="O31" s="6">
-        <v>1</v>
-      </c>
-      <c r="P31" s="6"/>
-      <c r="Q31" s="6" t="s">
+        <v>0.03</v>
+      </c>
+      <c r="P31" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q31" s="6"/>
+      <c r="R31" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="R31" s="6">
+      <c r="S31" s="6">
         <v>210</v>
       </c>
-      <c r="S31" s="6">
+      <c r="T31" s="6">
         <v>115</v>
       </c>
-      <c r="T31" s="6">
+      <c r="U31" s="6">
         <v>280</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>177</v>
       </c>
@@ -5056,42 +5179,45 @@
       <c r="G32" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="I32" s="4" t="s">
+      <c r="I32" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="J32" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="J32" s="3" t="s">
+      <c r="K32" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K32" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="L32" s="6">
+      <c r="L32" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M32" s="6">
         <v>6</v>
       </c>
-      <c r="M32" s="6">
-        <v>1</v>
-      </c>
       <c r="N32" s="6">
-        <v>0.03</v>
+        <v>1</v>
       </c>
       <c r="O32" s="6">
-        <v>1</v>
-      </c>
-      <c r="P32" s="6"/>
-      <c r="Q32" s="6" t="s">
+        <v>0.03</v>
+      </c>
+      <c r="P32" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q32" s="6"/>
+      <c r="R32" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="R32" s="6">
+      <c r="S32" s="6">
         <v>210</v>
       </c>
-      <c r="S32" s="6">
+      <c r="T32" s="6">
         <v>115</v>
       </c>
-      <c r="T32" s="6">
+      <c r="U32" s="6">
         <v>280</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>65</v>
       </c>
@@ -5111,42 +5237,43 @@
         <v>42</v>
       </c>
       <c r="G33" s="6"/>
-      <c r="I33" s="4" t="s">
+      <c r="I33" s="6"/>
+      <c r="J33" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="J33" s="3" t="s">
+      <c r="K33" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K33" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="L33" s="6">
+      <c r="L33" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M33" s="6">
         <v>6</v>
       </c>
-      <c r="M33" s="6">
-        <v>1</v>
-      </c>
       <c r="N33" s="6">
-        <v>0.03</v>
+        <v>1</v>
       </c>
       <c r="O33" s="6">
-        <v>1</v>
-      </c>
-      <c r="P33" s="6"/>
-      <c r="Q33" s="6" t="s">
+        <v>0.03</v>
+      </c>
+      <c r="P33" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q33" s="6"/>
+      <c r="R33" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="R33" s="6">
+      <c r="S33" s="6">
         <v>280</v>
       </c>
-      <c r="S33" s="6">
+      <c r="T33" s="6">
         <v>115</v>
       </c>
-      <c r="T33" s="6">
+      <c r="U33" s="6">
         <v>280</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>177</v>
       </c>
@@ -5168,42 +5295,45 @@
       <c r="G34" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="I34" s="4" t="s">
+      <c r="I34" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="J34" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="J34" s="3" t="s">
+      <c r="K34" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K34" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="L34" s="6">
+      <c r="L34" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M34" s="6">
         <v>6</v>
       </c>
-      <c r="M34" s="6">
-        <v>1</v>
-      </c>
       <c r="N34" s="6">
-        <v>0.03</v>
+        <v>1</v>
       </c>
       <c r="O34" s="6">
-        <v>1</v>
-      </c>
-      <c r="P34" s="6"/>
-      <c r="Q34" s="6" t="s">
+        <v>0.03</v>
+      </c>
+      <c r="P34" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q34" s="6"/>
+      <c r="R34" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="R34" s="6">
+      <c r="S34" s="6">
         <v>280</v>
       </c>
-      <c r="S34" s="6">
+      <c r="T34" s="6">
         <v>115</v>
       </c>
-      <c r="T34" s="6">
+      <c r="U34" s="6">
         <v>280</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E35" s="7"/>
     </row>
   </sheetData>
@@ -5221,23 +5351,23 @@
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.625" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="8.625" customWidth="1"/>
-    <col min="9" max="9" width="18.125" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="30.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="8.6640625" customWidth="1"/>
+    <col min="9" max="9" width="18.109375" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="12.44140625" hidden="1" customWidth="1"/>
     <col min="11" max="13" width="0" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="10.625" hidden="1" customWidth="1"/>
-    <col min="15" max="16" width="8.625" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="13.5" hidden="1" customWidth="1"/>
-    <col min="18" max="20" width="8.625" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" hidden="1" customWidth="1"/>
+    <col min="15" max="16" width="8.6640625" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="13.44140625" hidden="1" customWidth="1"/>
+    <col min="18" max="20" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="1" customFormat="1" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -5302,7 +5432,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="1" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" s="1" customFormat="1" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>33</v>
       </c>
@@ -5367,7 +5497,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>67</v>
       </c>
@@ -5423,7 +5553,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>67</v>
       </c>
@@ -5479,7 +5609,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>73</v>
       </c>
@@ -5535,7 +5665,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>73</v>
       </c>
@@ -5591,7 +5721,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>75</v>
       </c>
@@ -5647,7 +5777,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>75</v>
       </c>
@@ -5703,7 +5833,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>76</v>
       </c>
@@ -5759,7 +5889,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>76</v>
       </c>
@@ -5815,14 +5945,14 @@
         <v>476</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E11" s="7"/>
       <c r="G11" s="6"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="G12" s="6"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="G13" s="6"/>
     </row>
   </sheetData>
@@ -5840,13 +5970,13 @@
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>117</v>
       </c>
@@ -5869,7 +5999,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>118</v>
       </c>
@@ -5892,7 +6022,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>115</v>
       </c>
@@ -5904,7 +6034,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>119</v>
       </c>
@@ -5921,7 +6051,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>42</v>
       </c>
@@ -5944,7 +6074,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update PDS support files
</commit_message>
<xml_diff>
--- a/AutoLoader/Contents/Support/PowerDistributionSystem/LV_AC_CircuitBreaker_ImportLibrary_19DX101.xlsx
+++ b/AutoLoader/Contents/Support/PowerDistributionSystem/LV_AC_CircuitBreaker_ImportLibrary_19DX101.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="MCB" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="Trip Device" sheetId="15" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">ACB!$A$2:$T$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">ACB!$A$2:$T$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MCB!$A$2:$U$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">MCCB!$A$2:$U$3</definedName>
   </definedNames>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1205" uniqueCount="192">
   <si>
     <t>Trip Device</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -780,6 +780,14 @@
   </si>
   <si>
     <t>2.5;4;6;10;12.5;16;25;32;40;50;63</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3P+N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3P+N</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1138,10 +1146,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V34"/>
+  <dimension ref="A1:V42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U40" sqref="U40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1934,7 +1942,7 @@
         <v>0.23</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>50</v>
@@ -1995,7 +2003,7 @@
         <v>0.23</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>50</v>
@@ -2046,23 +2054,23 @@
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="6">
         <v>63</v>
       </c>
-      <c r="C15" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>128</v>
+      <c r="C15" s="6">
+        <v>0.23</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>112</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>36</v>
+        <v>50</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>35</v>
       </c>
       <c r="G15" s="6"/>
       <c r="H15" s="6" t="s">
@@ -2075,54 +2083,54 @@
       <c r="K15" s="3">
         <v>1</v>
       </c>
-      <c r="L15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O15" s="2">
-        <v>0.03</v>
-      </c>
-      <c r="P15" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q15" s="2">
+      <c r="L15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O15" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="P15" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="6">
         <v>35</v>
       </c>
-      <c r="R15" s="2" t="s">
+      <c r="R15" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="S15" s="2">
-        <v>54</v>
-      </c>
-      <c r="T15" s="2">
+      <c r="S15" s="6">
+        <v>36</v>
+      </c>
+      <c r="T15" s="6">
         <v>74</v>
       </c>
-      <c r="U15" s="2">
+      <c r="U15" s="6">
         <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="6">
         <v>63</v>
       </c>
-      <c r="C16" s="2">
-        <v>0.4</v>
+      <c r="C16" s="6">
+        <v>0.23</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="E16" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E16" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="6" t="s">
         <v>34</v>
       </c>
       <c r="G16" s="6"/>
@@ -2136,55 +2144,55 @@
       <c r="K16" s="3">
         <v>1</v>
       </c>
-      <c r="L16" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M16" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N16" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O16" s="2">
-        <v>0.03</v>
-      </c>
-      <c r="P16" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q16" s="2">
+      <c r="L16" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M16" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N16" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O16" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="P16" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="6">
         <v>35</v>
       </c>
-      <c r="R16" s="2" t="s">
+      <c r="R16" s="6" t="s">
         <v>15</v>
       </c>
       <c r="S16" s="6">
-        <v>54</v>
-      </c>
-      <c r="T16" s="2">
+        <v>36</v>
+      </c>
+      <c r="T16" s="6">
         <v>74</v>
       </c>
-      <c r="U16" s="2">
+      <c r="U16" s="6">
         <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="2">
         <v>63</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="2">
         <v>0.4</v>
       </c>
-      <c r="D17" s="6" t="s">
-        <v>129</v>
+      <c r="D17" s="2" t="s">
+        <v>128</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="F17" s="6" t="s">
-        <v>35</v>
+      <c r="F17" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="G17" s="6"/>
       <c r="H17" s="6" t="s">
@@ -2197,54 +2205,54 @@
       <c r="K17" s="3">
         <v>1</v>
       </c>
-      <c r="L17" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="M17" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="N17" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="O17" s="6">
-        <v>0.03</v>
-      </c>
-      <c r="P17" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q17" s="6">
+      <c r="L17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O17" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="P17" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="2">
         <v>35</v>
       </c>
-      <c r="R17" s="6" t="s">
+      <c r="R17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="S17" s="6">
-        <v>72</v>
-      </c>
-      <c r="T17" s="6">
+      <c r="S17" s="2">
+        <v>54</v>
+      </c>
+      <c r="T17" s="2">
         <v>74</v>
       </c>
-      <c r="U17" s="6">
+      <c r="U17" s="2">
         <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="2">
         <v>63</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="2">
         <v>0.4</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="E18" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="2" t="s">
         <v>34</v>
       </c>
       <c r="G18" s="6"/>
@@ -2258,79 +2266,75 @@
       <c r="K18" s="3">
         <v>1</v>
       </c>
-      <c r="L18" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="M18" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="N18" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="O18" s="6">
-        <v>0.03</v>
-      </c>
-      <c r="P18" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q18" s="6">
+      <c r="L18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O18" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="P18" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="2">
         <v>35</v>
       </c>
-      <c r="R18" s="6" t="s">
+      <c r="R18" s="2" t="s">
         <v>15</v>
       </c>
       <c r="S18" s="6">
-        <v>72</v>
-      </c>
-      <c r="T18" s="6">
+        <v>54</v>
+      </c>
+      <c r="T18" s="2">
         <v>74</v>
       </c>
-      <c r="U18" s="6">
+      <c r="U18" s="2">
         <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>88</v>
+        <v>39</v>
       </c>
       <c r="B19" s="6">
         <v>63</v>
       </c>
       <c r="C19" s="6">
-        <v>0.23</v>
+        <v>0.4</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>50</v>
+        <v>189</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>168</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="G19" s="6"/>
       <c r="H19" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="I19" s="6" t="s">
-        <v>186</v>
-      </c>
+      <c r="I19" s="6"/>
       <c r="J19" s="6" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="K19" s="3">
         <v>1</v>
       </c>
       <c r="L19" s="6" t="s">
-        <v>85</v>
+        <v>19</v>
       </c>
       <c r="M19" s="6" t="s">
-        <v>85</v>
+        <v>19</v>
       </c>
       <c r="N19" s="6" t="s">
-        <v>85</v>
+        <v>19</v>
       </c>
       <c r="O19" s="6">
         <v>0.03</v>
@@ -2342,10 +2346,10 @@
         <v>35</v>
       </c>
       <c r="R19" s="6" t="s">
-        <v>86</v>
+        <v>15</v>
       </c>
       <c r="S19" s="6">
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="T19" s="6">
         <v>74</v>
@@ -2356,34 +2360,30 @@
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>88</v>
+        <v>39</v>
       </c>
       <c r="B20" s="6">
         <v>63</v>
       </c>
       <c r="C20" s="6">
-        <v>0.23</v>
+        <v>0.4</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>50</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>168</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="G20" s="6"/>
       <c r="H20" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="I20" s="6" t="s">
-        <v>186</v>
-      </c>
+      <c r="I20" s="6"/>
       <c r="J20" s="6" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="K20" s="3">
         <v>1</v>
@@ -2410,7 +2410,7 @@
         <v>15</v>
       </c>
       <c r="S20" s="6">
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="T20" s="6">
         <v>74</v>
@@ -2421,7 +2421,7 @@
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>88</v>
+        <v>39</v>
       </c>
       <c r="B21" s="6">
         <v>63</v>
@@ -2430,25 +2430,21 @@
         <v>0.4</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>124</v>
+        <v>189</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>167</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="G21" s="6"/>
       <c r="H21" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="I21" s="6" t="s">
-        <v>186</v>
-      </c>
+      <c r="I21" s="6"/>
       <c r="J21" s="6" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="K21" s="3">
         <v>1</v>
@@ -2475,7 +2471,7 @@
         <v>15</v>
       </c>
       <c r="S21" s="6">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="T21" s="6">
         <v>74</v>
@@ -2486,7 +2482,7 @@
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>88</v>
+        <v>39</v>
       </c>
       <c r="B22" s="6">
         <v>63</v>
@@ -2495,37 +2491,33 @@
         <v>0.4</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>124</v>
+        <v>50</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>167</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="G22" s="6"/>
       <c r="H22" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="I22" s="6" t="s">
-        <v>186</v>
-      </c>
+      <c r="I22" s="6"/>
       <c r="J22" s="6" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="K22" s="3">
         <v>1</v>
       </c>
       <c r="L22" s="6" t="s">
-        <v>85</v>
+        <v>19</v>
       </c>
       <c r="M22" s="6" t="s">
-        <v>85</v>
+        <v>19</v>
       </c>
       <c r="N22" s="6" t="s">
-        <v>85</v>
+        <v>19</v>
       </c>
       <c r="O22" s="6">
         <v>0.03</v>
@@ -2537,7 +2529,7 @@
         <v>35</v>
       </c>
       <c r="R22" s="6" t="s">
-        <v>86</v>
+        <v>15</v>
       </c>
       <c r="S22" s="6">
         <v>72</v>
@@ -2551,10 +2543,10 @@
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>119</v>
+        <v>88</v>
       </c>
       <c r="B23" s="6">
-        <v>100</v>
+        <v>63</v>
       </c>
       <c r="C23" s="6">
         <v>0.23</v>
@@ -2563,22 +2555,22 @@
         <v>130</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>126</v>
+        <v>50</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>104</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>110</v>
+        <v>51</v>
       </c>
       <c r="I23" s="6" t="s">
         <v>186</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K23" s="3">
         <v>1</v>
@@ -2599,30 +2591,27 @@
         <v>1</v>
       </c>
       <c r="Q23" s="6">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="R23" s="6" t="s">
         <v>86</v>
       </c>
       <c r="S23" s="6">
-        <v>81</v>
+        <v>54</v>
       </c>
       <c r="T23" s="6">
         <v>74</v>
       </c>
       <c r="U23" s="6">
-        <v>105</v>
-      </c>
-      <c r="V23" s="6" t="s">
-        <v>178</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>119</v>
+        <v>88</v>
       </c>
       <c r="B24" s="6">
-        <v>100</v>
+        <v>63</v>
       </c>
       <c r="C24" s="6">
         <v>0.23</v>
@@ -2631,16 +2620,16 @@
         <v>131</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>126</v>
+        <v>50</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>104</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>110</v>
+        <v>51</v>
       </c>
       <c r="I24" s="6" t="s">
         <v>186</v>
@@ -2667,30 +2656,27 @@
         <v>1</v>
       </c>
       <c r="Q24" s="6">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="R24" s="6" t="s">
         <v>15</v>
       </c>
       <c r="S24" s="6">
-        <v>72</v>
+        <v>36</v>
       </c>
       <c r="T24" s="6">
         <v>74</v>
       </c>
       <c r="U24" s="6">
-        <v>105</v>
-      </c>
-      <c r="V24" s="6" t="s">
-        <v>178</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>119</v>
+        <v>88</v>
       </c>
       <c r="B25" s="6">
-        <v>100</v>
+        <v>63</v>
       </c>
       <c r="C25" s="6">
         <v>0.4</v>
@@ -2699,7 +2685,7 @@
         <v>132</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F25" s="6" t="s">
         <v>105</v>
@@ -2708,7 +2694,7 @@
         <v>167</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>110</v>
+        <v>51</v>
       </c>
       <c r="I25" s="6" t="s">
         <v>186</v>
@@ -2735,30 +2721,27 @@
         <v>1</v>
       </c>
       <c r="Q25" s="6">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="R25" s="6" t="s">
         <v>15</v>
       </c>
       <c r="S25" s="6">
-        <v>153</v>
+        <v>90</v>
       </c>
       <c r="T25" s="6">
         <v>74</v>
       </c>
       <c r="U25" s="6">
-        <v>105</v>
-      </c>
-      <c r="V25" s="6" t="s">
-        <v>178</v>
+        <v>82</v>
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>119</v>
+        <v>88</v>
       </c>
       <c r="B26" s="6">
-        <v>100</v>
+        <v>63</v>
       </c>
       <c r="C26" s="6">
         <v>0.4</v>
@@ -2767,7 +2750,7 @@
         <v>133</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>105</v>
@@ -2776,13 +2759,13 @@
         <v>167</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>110</v>
+        <v>51</v>
       </c>
       <c r="I26" s="6" t="s">
         <v>186</v>
       </c>
       <c r="J26" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="K26" s="3">
         <v>1</v>
@@ -2803,83 +2786,84 @@
         <v>1</v>
       </c>
       <c r="Q26" s="6">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="R26" s="6" t="s">
         <v>86</v>
       </c>
       <c r="S26" s="6">
-        <v>144</v>
+        <v>72</v>
       </c>
       <c r="T26" s="6">
         <v>74</v>
       </c>
       <c r="U26" s="6">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B27" s="6">
+        <v>100</v>
+      </c>
+      <c r="C27" s="6">
+        <v>0.23</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="J27" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="K27" s="3">
+        <v>1</v>
+      </c>
+      <c r="L27" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="M27" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="N27" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="O27" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="P27" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q27" s="6">
+        <v>50</v>
+      </c>
+      <c r="R27" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="S27" s="6">
+        <v>81</v>
+      </c>
+      <c r="T27" s="6">
+        <v>74</v>
+      </c>
+      <c r="U27" s="6">
         <v>105</v>
-      </c>
-      <c r="V26" s="6" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B27" s="2">
-        <v>125</v>
-      </c>
-      <c r="C27" s="2">
-        <v>0.23</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="I27" s="6"/>
-      <c r="J27" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="K27" s="3">
-        <v>1</v>
-      </c>
-      <c r="L27" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M27" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N27" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O27" s="2">
-        <v>0.03</v>
-      </c>
-      <c r="P27" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q27" s="2">
-        <v>50</v>
-      </c>
-      <c r="R27" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="S27" s="6">
-        <v>27</v>
-      </c>
-      <c r="T27" s="2">
-        <v>74</v>
-      </c>
-      <c r="U27" s="2">
-        <v>82</v>
       </c>
       <c r="V27" s="6" t="s">
         <v>178</v>
@@ -2887,30 +2871,34 @@
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>40</v>
+        <v>119</v>
       </c>
       <c r="B28" s="6">
-        <v>125</v>
+        <v>100</v>
       </c>
       <c r="C28" s="6">
         <v>0.23</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G28" s="6"/>
+        <v>104</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>167</v>
+      </c>
       <c r="H28" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="I28" s="6"/>
+        <v>110</v>
+      </c>
+      <c r="I28" s="6" t="s">
+        <v>186</v>
+      </c>
       <c r="J28" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="K28" s="3">
         <v>1</v>
@@ -2937,77 +2925,81 @@
         <v>15</v>
       </c>
       <c r="S28" s="6">
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="T28" s="6">
         <v>74</v>
       </c>
       <c r="U28" s="6">
-        <v>82</v>
+        <v>105</v>
       </c>
       <c r="V28" s="6" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B29" s="2">
+      <c r="A29" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B29" s="6">
+        <v>100</v>
+      </c>
+      <c r="C29" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="E29" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="C29" s="2">
-        <v>0.23</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G29" s="6"/>
+      <c r="F29" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>167</v>
+      </c>
       <c r="H29" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="I29" s="6"/>
+        <v>110</v>
+      </c>
+      <c r="I29" s="6" t="s">
+        <v>186</v>
+      </c>
       <c r="J29" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="K29" s="3">
         <v>1</v>
       </c>
-      <c r="L29" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M29" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N29" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O29" s="2">
-        <v>0.03</v>
-      </c>
-      <c r="P29" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q29" s="2">
+      <c r="L29" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M29" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N29" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O29" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="P29" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q29" s="6">
         <v>50</v>
       </c>
-      <c r="R29" s="2" t="s">
+      <c r="R29" s="6" t="s">
         <v>15</v>
       </c>
       <c r="S29" s="6">
-        <v>27</v>
-      </c>
-      <c r="T29" s="2">
+        <v>153</v>
+      </c>
+      <c r="T29" s="6">
         <v>74</v>
       </c>
-      <c r="U29" s="2">
-        <v>82</v>
+      <c r="U29" s="6">
+        <v>105</v>
       </c>
       <c r="V29" s="6" t="s">
         <v>178</v>
@@ -3015,42 +3007,46 @@
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>40</v>
+        <v>119</v>
       </c>
       <c r="B30" s="6">
+        <v>100</v>
+      </c>
+      <c r="C30" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="E30" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="C30" s="6">
-        <v>0.23</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>127</v>
-      </c>
       <c r="F30" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="G30" s="6"/>
+        <v>105</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>167</v>
+      </c>
       <c r="H30" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="I30" s="6"/>
+        <v>110</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>186</v>
+      </c>
       <c r="J30" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="K30" s="3">
         <v>1</v>
       </c>
       <c r="L30" s="6" t="s">
-        <v>19</v>
+        <v>85</v>
       </c>
       <c r="M30" s="6" t="s">
-        <v>19</v>
+        <v>85</v>
       </c>
       <c r="N30" s="6" t="s">
-        <v>19</v>
+        <v>85</v>
       </c>
       <c r="O30" s="6">
         <v>0.03</v>
@@ -3062,16 +3058,16 @@
         <v>50</v>
       </c>
       <c r="R30" s="6" t="s">
-        <v>15</v>
+        <v>86</v>
       </c>
       <c r="S30" s="6">
-        <v>54</v>
+        <v>144</v>
       </c>
       <c r="T30" s="6">
         <v>74</v>
       </c>
       <c r="U30" s="6">
-        <v>82</v>
+        <v>105</v>
       </c>
       <c r="V30" s="6" t="s">
         <v>178</v>
@@ -3085,17 +3081,18 @@
         <v>125</v>
       </c>
       <c r="C31" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="E31" s="6" t="s">
+        <v>0.23</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>127</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="G31" s="6"/>
       <c r="H31" s="6" t="s">
         <v>51</v>
       </c>
@@ -3128,7 +3125,7 @@
         <v>15</v>
       </c>
       <c r="S31" s="6">
-        <v>81</v>
+        <v>27</v>
       </c>
       <c r="T31" s="2">
         <v>74</v>
@@ -3148,10 +3145,10 @@
         <v>125</v>
       </c>
       <c r="C32" s="6">
-        <v>0.4</v>
+        <v>0.23</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>129</v>
+        <v>102</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>127</v>
@@ -3159,6 +3156,7 @@
       <c r="F32" s="6" t="s">
         <v>35</v>
       </c>
+      <c r="G32" s="6"/>
       <c r="H32" s="6" t="s">
         <v>51</v>
       </c>
@@ -3191,7 +3189,7 @@
         <v>15</v>
       </c>
       <c r="S32" s="6">
-        <v>108</v>
+        <v>54</v>
       </c>
       <c r="T32" s="6">
         <v>74</v>
@@ -3200,30 +3198,31 @@
         <v>82</v>
       </c>
       <c r="V32" s="6" t="s">
-        <v>178</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B33" s="6">
         <v>125</v>
       </c>
-      <c r="C33" s="2">
-        <v>0.4</v>
+      <c r="C33" s="6">
+        <v>0.23</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="F33" s="2" t="s">
-        <v>37</v>
-      </c>
+      <c r="F33" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G33" s="6"/>
       <c r="H33" s="6" t="s">
-        <v>109</v>
+        <v>51</v>
       </c>
       <c r="I33" s="6"/>
       <c r="J33" s="6" t="s">
@@ -3232,34 +3231,34 @@
       <c r="K33" s="3">
         <v>1</v>
       </c>
-      <c r="L33" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M33" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N33" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O33" s="2">
-        <v>0.03</v>
-      </c>
-      <c r="P33" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q33" s="2">
+      <c r="L33" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M33" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N33" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O33" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="P33" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q33" s="6">
         <v>50</v>
       </c>
-      <c r="R33" s="2" t="s">
+      <c r="R33" s="6" t="s">
         <v>15</v>
       </c>
       <c r="S33" s="6">
-        <v>81</v>
-      </c>
-      <c r="T33" s="2">
+        <v>54</v>
+      </c>
+      <c r="T33" s="6">
         <v>74</v>
       </c>
-      <c r="U33" s="2">
+      <c r="U33" s="6">
         <v>82</v>
       </c>
       <c r="V33" s="6" t="s">
@@ -3267,26 +3266,27 @@
       </c>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B34" s="6">
+      <c r="B34" s="2">
         <v>125</v>
       </c>
-      <c r="C34" s="6">
-        <v>0.4</v>
+      <c r="C34" s="2">
+        <v>0.23</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>129</v>
+        <v>101</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="F34" s="6" t="s">
-        <v>34</v>
-      </c>
+      <c r="F34" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G34" s="6"/>
       <c r="H34" s="6" t="s">
-        <v>109</v>
+        <v>51</v>
       </c>
       <c r="I34" s="6"/>
       <c r="J34" s="6" t="s">
@@ -3295,37 +3295,543 @@
       <c r="K34" s="3">
         <v>1</v>
       </c>
-      <c r="L34" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="M34" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="N34" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="O34" s="6">
-        <v>0.03</v>
-      </c>
-      <c r="P34" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q34" s="6">
+      <c r="L34" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M34" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N34" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O34" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="P34" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q34" s="2">
         <v>50</v>
       </c>
-      <c r="R34" s="6" t="s">
+      <c r="R34" s="2" t="s">
         <v>15</v>
       </c>
       <c r="S34" s="6">
+        <v>27</v>
+      </c>
+      <c r="T34" s="2">
+        <v>74</v>
+      </c>
+      <c r="U34" s="2">
+        <v>82</v>
+      </c>
+      <c r="V34" s="6" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35" s="6">
+        <v>125</v>
+      </c>
+      <c r="C35" s="6">
+        <v>0.23</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="K35" s="3">
+        <v>1</v>
+      </c>
+      <c r="L35" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M35" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N35" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O35" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="P35" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q35" s="6">
+        <v>50</v>
+      </c>
+      <c r="R35" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="S35" s="6">
+        <v>54</v>
+      </c>
+      <c r="T35" s="6">
+        <v>74</v>
+      </c>
+      <c r="U35" s="6">
+        <v>82</v>
+      </c>
+      <c r="V35" s="6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B36" s="6">
+        <v>125</v>
+      </c>
+      <c r="C36" s="6">
+        <v>0.23</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="I36" s="6"/>
+      <c r="J36" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="K36" s="3">
+        <v>1</v>
+      </c>
+      <c r="L36" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M36" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N36" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O36" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="P36" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q36" s="6">
+        <v>50</v>
+      </c>
+      <c r="R36" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="S36" s="6">
+        <v>54</v>
+      </c>
+      <c r="T36" s="6">
+        <v>74</v>
+      </c>
+      <c r="U36" s="6">
+        <v>82</v>
+      </c>
+      <c r="V36" s="6" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B37" s="2">
+        <v>125</v>
+      </c>
+      <c r="C37" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H37" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="I37" s="6"/>
+      <c r="J37" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="K37" s="3">
+        <v>1</v>
+      </c>
+      <c r="L37" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M37" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N37" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O37" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="P37" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q37" s="2">
+        <v>50</v>
+      </c>
+      <c r="R37" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="S37" s="6">
+        <v>81</v>
+      </c>
+      <c r="T37" s="2">
+        <v>74</v>
+      </c>
+      <c r="U37" s="2">
+        <v>82</v>
+      </c>
+      <c r="V37" s="6" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38" s="6">
+        <v>125</v>
+      </c>
+      <c r="C38" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H38" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="I38" s="6"/>
+      <c r="J38" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="K38" s="3">
+        <v>1</v>
+      </c>
+      <c r="L38" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M38" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N38" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O38" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="P38" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q38" s="6">
+        <v>50</v>
+      </c>
+      <c r="R38" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="S38" s="6">
         <v>108</v>
       </c>
-      <c r="T34" s="6">
+      <c r="T38" s="6">
         <v>74</v>
       </c>
-      <c r="U34" s="6">
+      <c r="U38" s="6">
         <v>82</v>
       </c>
-      <c r="V34" s="6" t="s">
+      <c r="V38" s="6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39" s="6">
+        <v>125</v>
+      </c>
+      <c r="C39" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H39" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="I39" s="6"/>
+      <c r="J39" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="K39" s="3">
+        <v>1</v>
+      </c>
+      <c r="L39" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M39" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N39" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O39" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="P39" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q39" s="6">
+        <v>50</v>
+      </c>
+      <c r="R39" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="S39" s="6">
+        <v>108</v>
+      </c>
+      <c r="T39" s="6">
+        <v>74</v>
+      </c>
+      <c r="U39" s="6">
+        <v>82</v>
+      </c>
+      <c r="V39" s="6" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" s="2">
+        <v>125</v>
+      </c>
+      <c r="C40" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H40" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="I40" s="6"/>
+      <c r="J40" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="K40" s="3">
+        <v>1</v>
+      </c>
+      <c r="L40" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M40" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N40" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O40" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="P40" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q40" s="2">
+        <v>50</v>
+      </c>
+      <c r="R40" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="S40" s="6">
+        <v>81</v>
+      </c>
+      <c r="T40" s="2">
+        <v>74</v>
+      </c>
+      <c r="U40" s="2">
+        <v>82</v>
+      </c>
+      <c r="V40" s="6" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41" s="6">
+        <v>125</v>
+      </c>
+      <c r="C41" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H41" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="I41" s="6"/>
+      <c r="J41" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="K41" s="3">
+        <v>1</v>
+      </c>
+      <c r="L41" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M41" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N41" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O41" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="P41" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q41" s="6">
+        <v>50</v>
+      </c>
+      <c r="R41" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="S41" s="6">
+        <v>108</v>
+      </c>
+      <c r="T41" s="6">
+        <v>74</v>
+      </c>
+      <c r="U41" s="6">
+        <v>82</v>
+      </c>
+      <c r="V41" s="6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B42" s="6">
+        <v>125</v>
+      </c>
+      <c r="C42" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H42" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="I42" s="6"/>
+      <c r="J42" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="K42" s="3">
+        <v>1</v>
+      </c>
+      <c r="L42" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M42" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N42" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O42" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="P42" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q42" s="6">
+        <v>50</v>
+      </c>
+      <c r="R42" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="S42" s="6">
+        <v>108</v>
+      </c>
+      <c r="T42" s="6">
+        <v>74</v>
+      </c>
+      <c r="U42" s="6">
+        <v>82</v>
+      </c>
+      <c r="V42" s="6" t="s">
         <v>178</v>
       </c>
     </row>
@@ -3339,10 +3845,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V35"/>
+  <dimension ref="A1:V51"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3742,16 +4248,17 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>139</v>
+        <v>191</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>188</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>136</v>
+        <v>35</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
       <c r="J7" s="4" t="s">
         <v>84</v>
       </c>
@@ -3798,16 +4305,17 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>139</v>
+        <v>191</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>82</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>137</v>
+        <v>34</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
       <c r="J8" s="4" t="s">
         <v>84</v>
       </c>
@@ -3854,7 +4362,7 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>139</v>
+        <v>191</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>54</v>
@@ -3864,6 +4372,7 @@
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
       <c r="J9" s="4" t="s">
         <v>52</v>
       </c>
@@ -3910,7 +4419,7 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>123</v>
+        <v>191</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>54</v>
@@ -3961,86 +4470,84 @@
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" s="2">
-        <v>160</v>
+      <c r="A11" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="6">
+        <v>100</v>
       </c>
       <c r="C11" s="6">
         <v>0.41499999999999998</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>35</v>
+      <c r="D11" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>136</v>
       </c>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
       <c r="J11" s="4" t="s">
-        <v>52</v>
+        <v>84</v>
       </c>
       <c r="K11" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="L11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O11" s="2">
-        <v>0.03</v>
-      </c>
-      <c r="P11" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="2" t="s">
+      <c r="L11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O11" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="P11" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6" t="s">
         <v>47</v>
       </c>
       <c r="S11" s="6">
-        <v>105</v>
-      </c>
-      <c r="T11" s="2">
+        <v>140</v>
+      </c>
+      <c r="T11" s="6">
         <v>86</v>
       </c>
-      <c r="U11" s="2">
+      <c r="U11" s="6">
         <v>161</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B12" s="6">
-        <v>160</v>
+        <v>100</v>
       </c>
       <c r="C12" s="6">
         <v>0.41499999999999998</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
       <c r="J12" s="4" t="s">
-        <v>52</v>
+        <v>84</v>
       </c>
       <c r="K12" s="3" t="s">
         <v>53</v>
@@ -4065,7 +4572,7 @@
         <v>47</v>
       </c>
       <c r="S12" s="6">
-        <v>105</v>
+        <v>140</v>
       </c>
       <c r="T12" s="6">
         <v>86</v>
@@ -4075,77 +4582,76 @@
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B13" s="2">
-        <v>160</v>
+      <c r="A13" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="6">
+        <v>100</v>
       </c>
       <c r="C13" s="6">
         <v>0.41499999999999998</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>141</v>
+      <c r="D13" s="6" t="s">
+        <v>139</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="F13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" s="6" t="s">
         <v>42</v>
       </c>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
       <c r="J13" s="4" t="s">
         <v>52</v>
       </c>
       <c r="K13" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="L13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O13" s="2">
-        <v>0.03</v>
-      </c>
-      <c r="P13" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q13" s="2"/>
-      <c r="R13" s="2" t="s">
+      <c r="L13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O13" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="P13" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6" t="s">
         <v>47</v>
       </c>
       <c r="S13" s="6">
-        <v>105</v>
-      </c>
-      <c r="T13" s="2">
+        <v>140</v>
+      </c>
+      <c r="T13" s="6">
         <v>86</v>
       </c>
-      <c r="U13" s="2">
+      <c r="U13" s="6">
         <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="B14" s="6">
-        <v>160</v>
+        <v>100</v>
       </c>
       <c r="C14" s="6">
         <v>0.41499999999999998</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>42</v>
@@ -4183,7 +4689,7 @@
         <v>47</v>
       </c>
       <c r="S14" s="6">
-        <v>105</v>
+        <v>140</v>
       </c>
       <c r="T14" s="6">
         <v>86</v>
@@ -4193,22 +4699,22 @@
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="2">
         <v>160</v>
       </c>
       <c r="C15" s="6">
         <v>0.41499999999999998</v>
       </c>
-      <c r="D15" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="E15" s="6" t="s">
+      <c r="D15" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="2" t="s">
         <v>35</v>
       </c>
       <c r="G15" s="6"/>
@@ -4220,32 +4726,32 @@
       <c r="K15" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="L15" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="M15" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="N15" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="O15" s="6">
-        <v>0.03</v>
-      </c>
-      <c r="P15" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q15" s="6"/>
-      <c r="R15" s="6" t="s">
+      <c r="L15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O15" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="P15" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2" t="s">
         <v>47</v>
       </c>
       <c r="S15" s="6">
-        <v>140</v>
-      </c>
-      <c r="T15" s="6">
+        <v>105</v>
+      </c>
+      <c r="T15" s="2">
         <v>86</v>
       </c>
-      <c r="U15" s="6">
+      <c r="U15" s="2">
         <v>161</v>
       </c>
     </row>
@@ -4260,7 +4766,7 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>83</v>
@@ -4297,7 +4803,7 @@
         <v>47</v>
       </c>
       <c r="S16" s="6">
-        <v>140</v>
+        <v>105</v>
       </c>
       <c r="T16" s="6">
         <v>86</v>
@@ -4307,22 +4813,22 @@
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="2">
         <v>160</v>
       </c>
       <c r="C17" s="6">
         <v>0.41499999999999998</v>
       </c>
-      <c r="D17" s="6" t="s">
-        <v>139</v>
+      <c r="D17" s="2" t="s">
+        <v>141</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F17" s="2" t="s">
         <v>42</v>
       </c>
       <c r="G17" s="6"/>
@@ -4334,38 +4840,38 @@
       <c r="K17" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="L17" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="M17" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="N17" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="O17" s="6">
-        <v>0.03</v>
-      </c>
-      <c r="P17" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q17" s="6"/>
-      <c r="R17" s="6" t="s">
+      <c r="L17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O17" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="P17" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2" t="s">
         <v>47</v>
       </c>
       <c r="S17" s="6">
-        <v>140</v>
-      </c>
-      <c r="T17" s="6">
+        <v>105</v>
+      </c>
+      <c r="T17" s="2">
         <v>86</v>
       </c>
-      <c r="U17" s="6">
+      <c r="U17" s="2">
         <v>161</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B18" s="6">
         <v>160</v>
@@ -4374,7 +4880,7 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>123</v>
+        <v>138</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>55</v>
@@ -4415,7 +4921,7 @@
         <v>47</v>
       </c>
       <c r="S18" s="6">
-        <v>140</v>
+        <v>105</v>
       </c>
       <c r="T18" s="6">
         <v>86</v>
@@ -4426,24 +4932,26 @@
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B19" s="6">
-        <v>250</v>
+        <v>160</v>
       </c>
       <c r="C19" s="6">
         <v>0.41499999999999998</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>140</v>
+        <v>191</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>57</v>
+        <v>83</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>80</v>
+        <v>35</v>
       </c>
       <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
       <c r="J19" s="4" t="s">
         <v>52</v>
       </c>
@@ -4470,7 +4978,7 @@
         <v>47</v>
       </c>
       <c r="S19" s="6">
-        <v>105</v>
+        <v>140</v>
       </c>
       <c r="T19" s="6">
         <v>86</v>
@@ -4481,24 +4989,26 @@
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B20" s="6">
-        <v>250</v>
+        <v>160</v>
       </c>
       <c r="C20" s="6">
         <v>0.41499999999999998</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>140</v>
+        <v>191</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>57</v>
+        <v>83</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>79</v>
+        <v>34</v>
       </c>
       <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
       <c r="J20" s="4" t="s">
         <v>52</v>
       </c>
@@ -4525,7 +5035,7 @@
         <v>47</v>
       </c>
       <c r="S20" s="6">
-        <v>105</v>
+        <v>140</v>
       </c>
       <c r="T20" s="6">
         <v>86</v>
@@ -4536,24 +5046,26 @@
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B21" s="6">
-        <v>250</v>
+        <v>160</v>
       </c>
       <c r="C21" s="6">
         <v>0.41499999999999998</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>141</v>
+        <v>191</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>42</v>
       </c>
       <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
       <c r="J21" s="4" t="s">
         <v>52</v>
       </c>
@@ -4580,7 +5092,7 @@
         <v>47</v>
       </c>
       <c r="S21" s="6">
-        <v>105</v>
+        <v>140</v>
       </c>
       <c r="T21" s="6">
         <v>86</v>
@@ -4591,19 +5103,19 @@
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B22" s="6">
-        <v>250</v>
+        <v>160</v>
       </c>
       <c r="C22" s="6">
         <v>0.41499999999999998</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>138</v>
+        <v>191</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>42</v>
@@ -4611,6 +5123,7 @@
       <c r="G22" s="6" t="s">
         <v>169</v>
       </c>
+      <c r="H22" s="6"/>
       <c r="I22" s="6" t="s">
         <v>186</v>
       </c>
@@ -4640,7 +5153,7 @@
         <v>47</v>
       </c>
       <c r="S22" s="6">
-        <v>105</v>
+        <v>140</v>
       </c>
       <c r="T22" s="6">
         <v>86</v>
@@ -4651,10 +5164,10 @@
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B23" s="6">
-        <v>250</v>
+        <v>160</v>
       </c>
       <c r="C23" s="6">
         <v>0.41499999999999998</v>
@@ -4663,12 +5176,13 @@
         <v>139</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>57</v>
+        <v>83</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>79</v>
+        <v>35</v>
       </c>
       <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
       <c r="I23" s="6"/>
       <c r="J23" s="4" t="s">
         <v>52</v>
@@ -4707,10 +5221,10 @@
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B24" s="6">
-        <v>250</v>
+        <v>160</v>
       </c>
       <c r="C24" s="6">
         <v>0.41499999999999998</v>
@@ -4719,12 +5233,13 @@
         <v>139</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>57</v>
+        <v>83</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>79</v>
+        <v>142</v>
       </c>
       <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
       <c r="I24" s="6"/>
       <c r="J24" s="4" t="s">
         <v>52</v>
@@ -4763,10 +5278,10 @@
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B25" s="6">
-        <v>250</v>
+        <v>160</v>
       </c>
       <c r="C25" s="6">
         <v>0.41499999999999998</v>
@@ -4775,12 +5290,13 @@
         <v>139</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>164</v>
+        <v>55</v>
       </c>
       <c r="F25" s="6" t="s">
         <v>42</v>
       </c>
       <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
       <c r="I25" s="6"/>
       <c r="J25" s="4" t="s">
         <v>52</v>
@@ -4819,10 +5335,10 @@
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B26" s="6">
-        <v>250</v>
+        <v>160</v>
       </c>
       <c r="C26" s="6">
         <v>0.41499999999999998</v>
@@ -4831,7 +5347,7 @@
         <v>123</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>164</v>
+        <v>55</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>42</v>
@@ -4839,6 +5355,7 @@
       <c r="G26" s="6" t="s">
         <v>169</v>
       </c>
+      <c r="H26" s="6"/>
       <c r="I26" s="6" t="s">
         <v>186</v>
       </c>
@@ -4879,27 +5396,26 @@
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B27" s="6">
-        <v>400</v>
+        <v>250</v>
       </c>
       <c r="C27" s="6">
         <v>0.41499999999999998</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>60</v>
+        <v>140</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>42</v>
+        <v>80</v>
       </c>
       <c r="G27" s="6"/>
-      <c r="I27" s="6"/>
       <c r="J27" s="4" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="K27" s="3" t="s">
         <v>53</v>
@@ -4907,11 +5423,11 @@
       <c r="L27" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="M27" s="6">
-        <v>5</v>
-      </c>
-      <c r="N27" s="6">
-        <v>1</v>
+      <c r="M27" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N27" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="O27" s="6">
         <v>0.03</v>
@@ -4924,42 +5440,37 @@
         <v>47</v>
       </c>
       <c r="S27" s="6">
-        <v>140</v>
+        <v>105</v>
       </c>
       <c r="T27" s="6">
-        <v>110</v>
+        <v>86</v>
       </c>
       <c r="U27" s="6">
-        <v>255</v>
+        <v>161</v>
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>174</v>
+        <v>56</v>
       </c>
       <c r="B28" s="6">
-        <v>400</v>
+        <v>250</v>
       </c>
       <c r="C28" s="6">
         <v>0.41499999999999998</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>60</v>
+        <v>140</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="G28" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="I28" s="6" t="s">
-        <v>186</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="G28" s="6"/>
       <c r="J28" s="4" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="K28" s="3" t="s">
         <v>53</v>
@@ -4967,11 +5478,11 @@
       <c r="L28" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="M28" s="6">
-        <v>5</v>
-      </c>
-      <c r="N28" s="6">
-        <v>1</v>
+      <c r="M28" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N28" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="O28" s="6">
         <v>0.03</v>
@@ -4984,38 +5495,37 @@
         <v>47</v>
       </c>
       <c r="S28" s="6">
-        <v>140</v>
+        <v>105</v>
       </c>
       <c r="T28" s="6">
-        <v>110</v>
+        <v>86</v>
       </c>
       <c r="U28" s="6">
-        <v>255</v>
+        <v>161</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B29" s="6">
-        <v>400</v>
+        <v>250</v>
       </c>
       <c r="C29" s="6">
         <v>0.41499999999999998</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>42</v>
       </c>
       <c r="G29" s="6"/>
-      <c r="I29" s="6"/>
       <c r="J29" s="4" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="K29" s="3" t="s">
         <v>53</v>
@@ -5023,11 +5533,11 @@
       <c r="L29" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="M29" s="6">
-        <v>5</v>
-      </c>
-      <c r="N29" s="6">
-        <v>1</v>
+      <c r="M29" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N29" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="O29" s="6">
         <v>0.03</v>
@@ -5040,30 +5550,30 @@
         <v>47</v>
       </c>
       <c r="S29" s="6">
-        <v>185</v>
+        <v>105</v>
       </c>
       <c r="T29" s="6">
-        <v>110</v>
+        <v>86</v>
       </c>
       <c r="U29" s="6">
-        <v>255</v>
+        <v>161</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B30" s="6">
-        <v>400</v>
+        <v>250</v>
       </c>
       <c r="C30" s="6">
         <v>0.41499999999999998</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>123</v>
+        <v>138</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F30" s="6" t="s">
         <v>42</v>
@@ -5075,7 +5585,7 @@
         <v>186</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="K30" s="3" t="s">
         <v>53</v>
@@ -5083,11 +5593,11 @@
       <c r="L30" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="M30" s="6">
-        <v>5</v>
-      </c>
-      <c r="N30" s="6">
-        <v>1</v>
+      <c r="M30" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N30" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="O30" s="6">
         <v>0.03</v>
@@ -5100,38 +5610,37 @@
         <v>47</v>
       </c>
       <c r="S30" s="6">
-        <v>185</v>
+        <v>105</v>
       </c>
       <c r="T30" s="6">
-        <v>110</v>
+        <v>86</v>
       </c>
       <c r="U30" s="6">
-        <v>255</v>
+        <v>161</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B31" s="6">
-        <v>630</v>
+        <v>250</v>
       </c>
       <c r="C31" s="6">
         <v>0.41499999999999998</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>66</v>
+        <v>191</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>42</v>
+        <v>79</v>
       </c>
       <c r="G31" s="6"/>
-      <c r="I31" s="6"/>
       <c r="J31" s="4" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="K31" s="3" t="s">
         <v>53</v>
@@ -5139,11 +5648,11 @@
       <c r="L31" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="M31" s="6">
-        <v>6</v>
-      </c>
-      <c r="N31" s="6">
-        <v>1</v>
+      <c r="M31" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N31" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="O31" s="6">
         <v>0.03</v>
@@ -5156,42 +5665,37 @@
         <v>47</v>
       </c>
       <c r="S31" s="6">
-        <v>210</v>
+        <v>140</v>
       </c>
       <c r="T31" s="6">
-        <v>115</v>
+        <v>86</v>
       </c>
       <c r="U31" s="6">
-        <v>280</v>
+        <v>161</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>176</v>
+        <v>56</v>
       </c>
       <c r="B32" s="6">
-        <v>630</v>
+        <v>250</v>
       </c>
       <c r="C32" s="6">
         <v>0.41499999999999998</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>66</v>
+        <v>191</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="G32" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="I32" s="6" t="s">
-        <v>186</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="G32" s="6"/>
       <c r="J32" s="4" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="K32" s="3" t="s">
         <v>53</v>
@@ -5199,11 +5703,11 @@
       <c r="L32" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="M32" s="6">
-        <v>6</v>
-      </c>
-      <c r="N32" s="6">
-        <v>1</v>
+      <c r="M32" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N32" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="O32" s="6">
         <v>0.03</v>
@@ -5216,38 +5720,37 @@
         <v>47</v>
       </c>
       <c r="S32" s="6">
-        <v>210</v>
+        <v>140</v>
       </c>
       <c r="T32" s="6">
-        <v>115</v>
+        <v>86</v>
       </c>
       <c r="U32" s="6">
-        <v>280</v>
+        <v>161</v>
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B33" s="6">
-        <v>630</v>
+        <v>250</v>
       </c>
       <c r="C33" s="6">
         <v>0.41499999999999998</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>139</v>
+        <v>191</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="F33" s="6" t="s">
         <v>42</v>
       </c>
       <c r="G33" s="6"/>
-      <c r="I33" s="6"/>
       <c r="J33" s="4" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="K33" s="3" t="s">
         <v>53</v>
@@ -5255,11 +5758,11 @@
       <c r="L33" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="M33" s="6">
-        <v>6</v>
-      </c>
-      <c r="N33" s="6">
-        <v>1</v>
+      <c r="M33" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N33" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="O33" s="6">
         <v>0.03</v>
@@ -5272,30 +5775,30 @@
         <v>47</v>
       </c>
       <c r="S33" s="6">
-        <v>280</v>
+        <v>140</v>
       </c>
       <c r="T33" s="6">
-        <v>115</v>
+        <v>86</v>
       </c>
       <c r="U33" s="6">
-        <v>280</v>
+        <v>161</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B34" s="6">
-        <v>630</v>
+        <v>250</v>
       </c>
       <c r="C34" s="6">
         <v>0.41499999999999998</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>123</v>
+        <v>191</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="F34" s="6" t="s">
         <v>42</v>
@@ -5307,7 +5810,7 @@
         <v>186</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="K34" s="3" t="s">
         <v>53</v>
@@ -5315,11 +5818,11 @@
       <c r="L34" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="M34" s="6">
-        <v>6</v>
-      </c>
-      <c r="N34" s="6">
-        <v>1</v>
+      <c r="M34" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N34" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="O34" s="6">
         <v>0.03</v>
@@ -5332,17 +5835,941 @@
         <v>47</v>
       </c>
       <c r="S34" s="6">
+        <v>140</v>
+      </c>
+      <c r="T34" s="6">
+        <v>86</v>
+      </c>
+      <c r="U34" s="6">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B35" s="6">
+        <v>250</v>
+      </c>
+      <c r="C35" s="6">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="G35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="K35" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="L35" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M35" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N35" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O35" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="P35" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q35" s="6"/>
+      <c r="R35" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="S35" s="6">
+        <v>140</v>
+      </c>
+      <c r="T35" s="6">
+        <v>86</v>
+      </c>
+      <c r="U35" s="6">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36" s="6">
+        <v>250</v>
+      </c>
+      <c r="C36" s="6">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="G36" s="6"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="K36" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="L36" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M36" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N36" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O36" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="P36" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q36" s="6"/>
+      <c r="R36" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="S36" s="6">
+        <v>140</v>
+      </c>
+      <c r="T36" s="6">
+        <v>86</v>
+      </c>
+      <c r="U36" s="6">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B37" s="6">
+        <v>250</v>
+      </c>
+      <c r="C37" s="6">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G37" s="6"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="K37" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="L37" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M37" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N37" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O37" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="P37" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q37" s="6"/>
+      <c r="R37" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="S37" s="6">
+        <v>140</v>
+      </c>
+      <c r="T37" s="6">
+        <v>86</v>
+      </c>
+      <c r="U37" s="6">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="B38" s="6">
+        <v>250</v>
+      </c>
+      <c r="C38" s="6">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="I38" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="J38" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="K38" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="L38" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M38" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N38" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O38" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="P38" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q38" s="6"/>
+      <c r="R38" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="S38" s="6">
+        <v>140</v>
+      </c>
+      <c r="T38" s="6">
+        <v>86</v>
+      </c>
+      <c r="U38" s="6">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B39" s="6">
+        <v>400</v>
+      </c>
+      <c r="C39" s="6">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G39" s="6"/>
+      <c r="I39" s="6"/>
+      <c r="J39" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="K39" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="L39" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M39" s="6">
+        <v>5</v>
+      </c>
+      <c r="N39" s="6">
+        <v>1</v>
+      </c>
+      <c r="O39" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="P39" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q39" s="6"/>
+      <c r="R39" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="S39" s="6">
+        <v>140</v>
+      </c>
+      <c r="T39" s="6">
+        <v>110</v>
+      </c>
+      <c r="U39" s="6">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="B40" s="6">
+        <v>400</v>
+      </c>
+      <c r="C40" s="6">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G40" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="I40" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="J40" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="K40" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="L40" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M40" s="6">
+        <v>5</v>
+      </c>
+      <c r="N40" s="6">
+        <v>1</v>
+      </c>
+      <c r="O40" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="P40" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q40" s="6"/>
+      <c r="R40" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="S40" s="6">
+        <v>140</v>
+      </c>
+      <c r="T40" s="6">
+        <v>110</v>
+      </c>
+      <c r="U40" s="6">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B41" s="6">
+        <v>400</v>
+      </c>
+      <c r="C41" s="6">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G41" s="6"/>
+      <c r="I41" s="6"/>
+      <c r="J41" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="K41" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="L41" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M41" s="6">
+        <v>5</v>
+      </c>
+      <c r="N41" s="6">
+        <v>1</v>
+      </c>
+      <c r="O41" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="P41" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q41" s="6"/>
+      <c r="R41" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="S41" s="6">
+        <v>185</v>
+      </c>
+      <c r="T41" s="6">
+        <v>110</v>
+      </c>
+      <c r="U41" s="6">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="B42" s="6">
+        <v>400</v>
+      </c>
+      <c r="C42" s="6">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G42" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="I42" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="J42" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="K42" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="L42" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M42" s="6">
+        <v>5</v>
+      </c>
+      <c r="N42" s="6">
+        <v>1</v>
+      </c>
+      <c r="O42" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="P42" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q42" s="6"/>
+      <c r="R42" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="S42" s="6">
+        <v>185</v>
+      </c>
+      <c r="T42" s="6">
+        <v>110</v>
+      </c>
+      <c r="U42" s="6">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B43" s="6">
+        <v>400</v>
+      </c>
+      <c r="C43" s="6">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G43" s="6"/>
+      <c r="I43" s="6"/>
+      <c r="J43" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="K43" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="L43" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M43" s="6">
+        <v>5</v>
+      </c>
+      <c r="N43" s="6">
+        <v>1</v>
+      </c>
+      <c r="O43" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="P43" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q43" s="6"/>
+      <c r="R43" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="S43" s="6">
+        <v>185</v>
+      </c>
+      <c r="T43" s="6">
+        <v>110</v>
+      </c>
+      <c r="U43" s="6">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="B44" s="6">
+        <v>400</v>
+      </c>
+      <c r="C44" s="6">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G44" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="I44" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="J44" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="K44" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="L44" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M44" s="6">
+        <v>5</v>
+      </c>
+      <c r="N44" s="6">
+        <v>1</v>
+      </c>
+      <c r="O44" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="P44" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q44" s="6"/>
+      <c r="R44" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="S44" s="6">
+        <v>185</v>
+      </c>
+      <c r="T44" s="6">
+        <v>110</v>
+      </c>
+      <c r="U44" s="6">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B45" s="6">
+        <v>630</v>
+      </c>
+      <c r="C45" s="6">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G45" s="6"/>
+      <c r="I45" s="6"/>
+      <c r="J45" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="K45" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="L45" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M45" s="6">
+        <v>6</v>
+      </c>
+      <c r="N45" s="6">
+        <v>1</v>
+      </c>
+      <c r="O45" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="P45" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q45" s="6"/>
+      <c r="R45" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="S45" s="6">
+        <v>210</v>
+      </c>
+      <c r="T45" s="6">
+        <v>115</v>
+      </c>
+      <c r="U45" s="6">
         <v>280</v>
       </c>
-      <c r="T34" s="6">
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A46" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="B46" s="6">
+        <v>630</v>
+      </c>
+      <c r="C46" s="6">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G46" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="I46" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="J46" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="K46" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="L46" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M46" s="6">
+        <v>6</v>
+      </c>
+      <c r="N46" s="6">
+        <v>1</v>
+      </c>
+      <c r="O46" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="P46" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q46" s="6"/>
+      <c r="R46" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="S46" s="6">
+        <v>210</v>
+      </c>
+      <c r="T46" s="6">
         <v>115</v>
       </c>
-      <c r="U34" s="6">
+      <c r="U46" s="6">
         <v>280</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="E35" s="7"/>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A47" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B47" s="6">
+        <v>630</v>
+      </c>
+      <c r="C47" s="6">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G47" s="6"/>
+      <c r="I47" s="6"/>
+      <c r="J47" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="K47" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="L47" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M47" s="6">
+        <v>6</v>
+      </c>
+      <c r="N47" s="6">
+        <v>1</v>
+      </c>
+      <c r="O47" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="P47" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q47" s="6"/>
+      <c r="R47" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="S47" s="6">
+        <v>280</v>
+      </c>
+      <c r="T47" s="6">
+        <v>115</v>
+      </c>
+      <c r="U47" s="6">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A48" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="B48" s="6">
+        <v>630</v>
+      </c>
+      <c r="C48" s="6">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G48" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="I48" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="J48" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="K48" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="L48" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M48" s="6">
+        <v>6</v>
+      </c>
+      <c r="N48" s="6">
+        <v>1</v>
+      </c>
+      <c r="O48" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="P48" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q48" s="6"/>
+      <c r="R48" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="S48" s="6">
+        <v>280</v>
+      </c>
+      <c r="T48" s="6">
+        <v>115</v>
+      </c>
+      <c r="U48" s="6">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A49" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B49" s="6">
+        <v>630</v>
+      </c>
+      <c r="C49" s="6">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G49" s="6"/>
+      <c r="I49" s="6"/>
+      <c r="J49" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="K49" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="L49" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M49" s="6">
+        <v>6</v>
+      </c>
+      <c r="N49" s="6">
+        <v>1</v>
+      </c>
+      <c r="O49" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="P49" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q49" s="6"/>
+      <c r="R49" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="S49" s="6">
+        <v>280</v>
+      </c>
+      <c r="T49" s="6">
+        <v>115</v>
+      </c>
+      <c r="U49" s="6">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A50" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="B50" s="6">
+        <v>630</v>
+      </c>
+      <c r="C50" s="6">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G50" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="I50" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="J50" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="K50" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="L50" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M50" s="6">
+        <v>6</v>
+      </c>
+      <c r="N50" s="6">
+        <v>1</v>
+      </c>
+      <c r="O50" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="P50" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q50" s="6"/>
+      <c r="R50" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="S50" s="6">
+        <v>280</v>
+      </c>
+      <c r="T50" s="6">
+        <v>115</v>
+      </c>
+      <c r="U50" s="6">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="E51" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -5353,10 +6780,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U13"/>
+  <dimension ref="A1:U17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T14" sqref="T14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -5572,7 +6999,7 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>143</v>
+        <v>191</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>68</v>
@@ -5619,19 +7046,19 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B5" s="6">
-        <v>2000</v>
+        <v>1600</v>
       </c>
       <c r="C5" s="6">
         <v>0.41499999999999998</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>42</v>
@@ -5664,13 +7091,13 @@
         <v>72</v>
       </c>
       <c r="R5" s="6">
-        <v>347</v>
+        <v>318</v>
       </c>
       <c r="S5" s="6">
-        <v>395</v>
+        <v>297</v>
       </c>
       <c r="T5" s="6">
-        <v>438</v>
+        <v>352</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
@@ -5684,7 +7111,7 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>74</v>
@@ -5720,7 +7147,7 @@
         <v>72</v>
       </c>
       <c r="R6" s="6">
-        <v>442</v>
+        <v>347</v>
       </c>
       <c r="S6" s="6">
         <v>395</v>
@@ -5731,19 +7158,19 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B7" s="6">
-        <v>4000</v>
+        <v>2000</v>
       </c>
       <c r="C7" s="6">
         <v>0.41499999999999998</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>141</v>
+        <v>191</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>166</v>
+        <v>74</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>42</v>
@@ -5776,7 +7203,7 @@
         <v>72</v>
       </c>
       <c r="R7" s="6">
-        <v>401</v>
+        <v>442</v>
       </c>
       <c r="S7" s="6">
         <v>395</v>
@@ -5787,10 +7214,10 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B8" s="6">
-        <v>4000</v>
+        <v>2000</v>
       </c>
       <c r="C8" s="6">
         <v>0.41499999999999998</v>
@@ -5799,7 +7226,7 @@
         <v>143</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>165</v>
+        <v>74</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>42</v>
@@ -5832,7 +7259,7 @@
         <v>72</v>
       </c>
       <c r="R8" s="6">
-        <v>514</v>
+        <v>442</v>
       </c>
       <c r="S8" s="6">
         <v>395</v>
@@ -5843,19 +7270,19 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B9" s="6">
-        <v>6300</v>
+        <v>4000</v>
       </c>
       <c r="C9" s="6">
         <v>0.41499999999999998</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>77</v>
+        <v>166</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>42</v>
@@ -5863,7 +7290,7 @@
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
       <c r="I9" s="4" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="J9" s="3" t="s">
         <v>71</v>
@@ -5888,30 +7315,30 @@
         <v>72</v>
       </c>
       <c r="R9" s="6">
-        <v>754</v>
+        <v>401</v>
       </c>
       <c r="S9" s="6">
         <v>395</v>
       </c>
       <c r="T9" s="6">
-        <v>476</v>
+        <v>438</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B10" s="6">
-        <v>6300</v>
+        <v>4000</v>
       </c>
       <c r="C10" s="6">
         <v>0.41499999999999998</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>145</v>
+        <v>191</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>77</v>
+        <v>165</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>42</v>
@@ -5919,7 +7346,7 @@
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="4" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>71</v>
@@ -5944,24 +7371,248 @@
         <v>72</v>
       </c>
       <c r="R10" s="6">
-        <v>980</v>
+        <v>514</v>
       </c>
       <c r="S10" s="6">
         <v>395</v>
       </c>
       <c r="T10" s="6">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" s="6">
+        <v>4000</v>
+      </c>
+      <c r="C11" s="6">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N11" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="O11" s="6">
+        <v>1</v>
+      </c>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="R11" s="6">
+        <v>514</v>
+      </c>
+      <c r="S11" s="6">
+        <v>395</v>
+      </c>
+      <c r="T11" s="6">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" s="6">
+        <v>6300</v>
+      </c>
+      <c r="C12" s="6">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N12" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="O12" s="6">
+        <v>1</v>
+      </c>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="R12" s="6">
+        <v>754</v>
+      </c>
+      <c r="S12" s="6">
+        <v>395</v>
+      </c>
+      <c r="T12" s="6">
         <v>476</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="E11" s="7"/>
-      <c r="G11" s="6"/>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="G12" s="6"/>
-    </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B13" s="6">
+        <v>6300</v>
+      </c>
+      <c r="C13" s="6">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>42</v>
+      </c>
       <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N13" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="O13" s="6">
+        <v>1</v>
+      </c>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="R13" s="6">
+        <v>980</v>
+      </c>
+      <c r="S13" s="6">
+        <v>395</v>
+      </c>
+      <c r="T13" s="6">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" s="6">
+        <v>6300</v>
+      </c>
+      <c r="C14" s="6">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L14" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M14" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N14" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="O14" s="6">
+        <v>1</v>
+      </c>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="R14" s="6">
+        <v>980</v>
+      </c>
+      <c r="S14" s="6">
+        <v>395</v>
+      </c>
+      <c r="T14" s="6">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="E15" s="7"/>
+      <c r="G15" s="6"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="G16" s="6"/>
+    </row>
+    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G17" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Update PDS template file
</commit_message>
<xml_diff>
--- a/AutoLoader/Contents/Support/PowerDistributionSystem/LV_AC_CircuitBreaker_ImportLibrary_19DX101.xlsx
+++ b/AutoLoader/Contents/Support/PowerDistributionSystem/LV_AC_CircuitBreaker_ImportLibrary_19DX101.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="MCB" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1213" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1213" uniqueCount="191">
   <si>
     <t>Trip Device</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -318,14 +318,6 @@
   </si>
   <si>
     <t>100;150</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MA;TM</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MA;TM</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1178,7 +1170,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
@@ -1190,19 +1182,19 @@
         <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>45</v>
@@ -1238,7 +1230,7 @@
         <v>14</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:22" s="1" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
@@ -1261,16 +1253,16 @@
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>46</v>
@@ -1306,7 +1298,7 @@
         <v>32</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
@@ -1320,21 +1312,21 @@
         <v>0.23</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>35</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="K3" s="3">
         <v>1</v>
@@ -1370,7 +1362,7 @@
         <v>77</v>
       </c>
       <c r="V3" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.2">
@@ -1384,7 +1376,7 @@
         <v>0.23</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>49</v>
@@ -1394,7 +1386,7 @@
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="2" t="s">
@@ -1434,7 +1426,7 @@
         <v>77</v>
       </c>
       <c r="V4" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.2">
@@ -1448,7 +1440,7 @@
         <v>0.23</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>49</v>
@@ -1458,7 +1450,7 @@
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I5" s="6"/>
       <c r="J5" s="6" t="s">
@@ -1498,7 +1490,7 @@
         <v>77</v>
       </c>
       <c r="V5" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.2">
@@ -1512,7 +1504,7 @@
         <v>0.23</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>49</v>
@@ -1522,11 +1514,11 @@
       </c>
       <c r="G6" s="6"/>
       <c r="H6" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="K6" s="3">
         <v>1</v>
@@ -1562,12 +1554,12 @@
         <v>77</v>
       </c>
       <c r="V6" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B7" s="6">
         <v>32</v>
@@ -1576,37 +1568,37 @@
         <v>0.23</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>49</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="K7" s="3">
         <v>1</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="O7" s="6">
         <v>0.03</v>
@@ -1618,7 +1610,7 @@
         <v>10</v>
       </c>
       <c r="R7" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="S7" s="6">
         <v>54</v>
@@ -1630,12 +1622,12 @@
         <v>77</v>
       </c>
       <c r="V7" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B8" s="6">
         <v>32</v>
@@ -1644,25 +1636,25 @@
         <v>0.23</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>49</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="K8" s="3">
         <v>1</v>
@@ -1698,12 +1690,12 @@
         <v>77</v>
       </c>
       <c r="V8" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B9" s="6">
         <v>32</v>
@@ -1712,37 +1704,37 @@
         <v>0.4</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>49</v>
       </c>
       <c r="F9" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="J9" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="G9" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>101</v>
-      </c>
       <c r="K9" s="3">
         <v>1</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="N9" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="O9" s="6">
         <v>0.03</v>
@@ -1754,7 +1746,7 @@
         <v>10</v>
       </c>
       <c r="R9" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="S9" s="6">
         <v>90</v>
@@ -1766,12 +1758,12 @@
         <v>77</v>
       </c>
       <c r="V9" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B10" s="6">
         <v>32</v>
@@ -1780,25 +1772,25 @@
         <v>0.4</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>49</v>
       </c>
       <c r="F10" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="J10" s="6" t="s">
         <v>99</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>101</v>
       </c>
       <c r="K10" s="3">
         <v>1</v>
@@ -1834,7 +1826,7 @@
         <v>77</v>
       </c>
       <c r="V10" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.2">
@@ -1848,7 +1840,7 @@
         <v>0.23</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>50</v>
@@ -1862,7 +1854,7 @@
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K11" s="3">
         <v>1</v>
@@ -1909,7 +1901,7 @@
         <v>0.23</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>50</v>
@@ -1923,7 +1915,7 @@
       </c>
       <c r="I12" s="6"/>
       <c r="J12" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K12" s="3">
         <v>1</v>
@@ -1970,7 +1962,7 @@
         <v>0.23</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>50</v>
@@ -1984,7 +1976,7 @@
       </c>
       <c r="I13" s="6"/>
       <c r="J13" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K13" s="3">
         <v>1</v>
@@ -2031,7 +2023,7 @@
         <v>0.23</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>50</v>
@@ -2045,7 +2037,7 @@
       </c>
       <c r="I14" s="6"/>
       <c r="J14" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K14" s="3">
         <v>1</v>
@@ -2092,7 +2084,7 @@
         <v>0.23</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>50</v>
@@ -2106,7 +2098,7 @@
       </c>
       <c r="I15" s="6"/>
       <c r="J15" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K15" s="3">
         <v>1</v>
@@ -2153,7 +2145,7 @@
         <v>0.23</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>50</v>
@@ -2167,7 +2159,7 @@
       </c>
       <c r="I16" s="6"/>
       <c r="J16" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K16" s="3">
         <v>1</v>
@@ -2214,10 +2206,10 @@
         <v>0.4</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>36</v>
@@ -2228,7 +2220,7 @@
       </c>
       <c r="I17" s="6"/>
       <c r="J17" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K17" s="3">
         <v>1</v>
@@ -2275,7 +2267,7 @@
         <v>0.4</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>50</v>
@@ -2289,7 +2281,7 @@
       </c>
       <c r="I18" s="6"/>
       <c r="J18" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K18" s="3">
         <v>1</v>
@@ -2336,10 +2328,10 @@
         <v>0.4</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>35</v>
@@ -2350,7 +2342,7 @@
       </c>
       <c r="I19" s="6"/>
       <c r="J19" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K19" s="3">
         <v>1</v>
@@ -2397,7 +2389,7 @@
         <v>0.4</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>50</v>
@@ -2411,7 +2403,7 @@
       </c>
       <c r="I20" s="6"/>
       <c r="J20" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K20" s="3">
         <v>1</v>
@@ -2458,10 +2450,10 @@
         <v>0.4</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>35</v>
@@ -2472,7 +2464,7 @@
       </c>
       <c r="I21" s="6"/>
       <c r="J21" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K21" s="3">
         <v>1</v>
@@ -2519,7 +2511,7 @@
         <v>0.4</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>50</v>
@@ -2533,7 +2525,7 @@
       </c>
       <c r="I22" s="6"/>
       <c r="J22" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K22" s="3">
         <v>1</v>
@@ -2571,7 +2563,7 @@
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B23" s="6">
         <v>63</v>
@@ -2580,37 +2572,37 @@
         <v>0.23</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>50</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="H23" s="6" t="s">
         <v>51</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K23" s="3">
         <v>1</v>
       </c>
       <c r="L23" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M23" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="N23" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="O23" s="6">
         <v>0.03</v>
@@ -2622,7 +2614,7 @@
         <v>35</v>
       </c>
       <c r="R23" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="S23" s="6">
         <v>54</v>
@@ -2636,7 +2628,7 @@
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B24" s="6">
         <v>63</v>
@@ -2645,25 +2637,25 @@
         <v>0.23</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>50</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="H24" s="6" t="s">
         <v>51</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J24" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="K24" s="3">
         <v>1</v>
@@ -2701,7 +2693,7 @@
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B25" s="6">
         <v>63</v>
@@ -2710,25 +2702,25 @@
         <v>0.4</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H25" s="6" t="s">
         <v>51</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="K25" s="3">
         <v>1</v>
@@ -2766,7 +2758,7 @@
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B26" s="6">
         <v>63</v>
@@ -2775,37 +2767,37 @@
         <v>0.4</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H26" s="6" t="s">
         <v>51</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J26" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="K26" s="3">
         <v>1</v>
       </c>
       <c r="L26" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M26" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="N26" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="O26" s="6">
         <v>0.03</v>
@@ -2817,7 +2809,7 @@
         <v>35</v>
       </c>
       <c r="R26" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="S26" s="6">
         <v>72</v>
@@ -2831,7 +2823,7 @@
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B27" s="6">
         <v>100</v>
@@ -2840,37 +2832,37 @@
         <v>0.23</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="K27" s="3">
         <v>1</v>
       </c>
       <c r="L27" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M27" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="N27" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="O27" s="6">
         <v>0.03</v>
@@ -2882,7 +2874,7 @@
         <v>50</v>
       </c>
       <c r="R27" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="S27" s="6">
         <v>81</v>
@@ -2894,12 +2886,12 @@
         <v>105</v>
       </c>
       <c r="V27" s="6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B28" s="6">
         <v>100</v>
@@ -2908,25 +2900,25 @@
         <v>0.23</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J28" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="K28" s="3">
         <v>1</v>
@@ -2962,12 +2954,12 @@
         <v>105</v>
       </c>
       <c r="V28" s="6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B29" s="6">
         <v>100</v>
@@ -2976,25 +2968,25 @@
         <v>0.4</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J29" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="K29" s="3">
         <v>1</v>
@@ -3030,12 +3022,12 @@
         <v>105</v>
       </c>
       <c r="V29" s="6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B30" s="6">
         <v>100</v>
@@ -3044,37 +3036,37 @@
         <v>0.4</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="K30" s="3">
         <v>1</v>
       </c>
       <c r="L30" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M30" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="N30" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="O30" s="6">
         <v>0.03</v>
@@ -3086,7 +3078,7 @@
         <v>50</v>
       </c>
       <c r="R30" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="S30" s="6">
         <v>144</v>
@@ -3098,7 +3090,7 @@
         <v>105</v>
       </c>
       <c r="V30" s="6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.2">
@@ -3112,10 +3104,10 @@
         <v>0.23</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>35</v>
@@ -3126,7 +3118,7 @@
       </c>
       <c r="I31" s="6"/>
       <c r="J31" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K31" s="3">
         <v>1</v>
@@ -3162,7 +3154,7 @@
         <v>82</v>
       </c>
       <c r="V31" s="6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.2">
@@ -3176,10 +3168,10 @@
         <v>0.23</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F32" s="6" t="s">
         <v>35</v>
@@ -3190,7 +3182,7 @@
       </c>
       <c r="I32" s="6"/>
       <c r="J32" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K32" s="3">
         <v>1</v>
@@ -3226,7 +3218,7 @@
         <v>82</v>
       </c>
       <c r="V32" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.2">
@@ -3240,10 +3232,10 @@
         <v>0.23</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F33" s="6" t="s">
         <v>35</v>
@@ -3254,7 +3246,7 @@
       </c>
       <c r="I33" s="6"/>
       <c r="J33" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K33" s="3">
         <v>1</v>
@@ -3290,7 +3282,7 @@
         <v>82</v>
       </c>
       <c r="V33" s="6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.2">
@@ -3304,10 +3296,10 @@
         <v>0.23</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>37</v>
@@ -3318,7 +3310,7 @@
       </c>
       <c r="I34" s="6"/>
       <c r="J34" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K34" s="3">
         <v>1</v>
@@ -3354,7 +3346,7 @@
         <v>82</v>
       </c>
       <c r="V34" s="6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.2">
@@ -3368,10 +3360,10 @@
         <v>0.23</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F35" s="6" t="s">
         <v>34</v>
@@ -3382,7 +3374,7 @@
       </c>
       <c r="I35" s="6"/>
       <c r="J35" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K35" s="3">
         <v>1</v>
@@ -3418,7 +3410,7 @@
         <v>82</v>
       </c>
       <c r="V35" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.2">
@@ -3432,10 +3424,10 @@
         <v>0.23</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F36" s="6" t="s">
         <v>34</v>
@@ -3446,7 +3438,7 @@
       </c>
       <c r="I36" s="6"/>
       <c r="J36" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K36" s="3">
         <v>1</v>
@@ -3482,7 +3474,7 @@
         <v>82</v>
       </c>
       <c r="V36" s="6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.2">
@@ -3496,10 +3488,10 @@
         <v>0.4</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>35</v>
@@ -3509,7 +3501,7 @@
       </c>
       <c r="I37" s="6"/>
       <c r="J37" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K37" s="3">
         <v>1</v>
@@ -3545,7 +3537,7 @@
         <v>82</v>
       </c>
       <c r="V37" s="6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.2">
@@ -3559,10 +3551,10 @@
         <v>0.4</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F38" s="6" t="s">
         <v>35</v>
@@ -3572,7 +3564,7 @@
       </c>
       <c r="I38" s="6"/>
       <c r="J38" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K38" s="3">
         <v>1</v>
@@ -3608,7 +3600,7 @@
         <v>82</v>
       </c>
       <c r="V38" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.2">
@@ -3622,10 +3614,10 @@
         <v>0.4</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>35</v>
@@ -3635,7 +3627,7 @@
       </c>
       <c r="I39" s="6"/>
       <c r="J39" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K39" s="3">
         <v>1</v>
@@ -3671,7 +3663,7 @@
         <v>82</v>
       </c>
       <c r="V39" s="6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.2">
@@ -3685,20 +3677,20 @@
         <v>0.4</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>37</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I40" s="6"/>
       <c r="J40" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K40" s="3">
         <v>1</v>
@@ -3734,7 +3726,7 @@
         <v>82</v>
       </c>
       <c r="V40" s="6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.2">
@@ -3748,20 +3740,20 @@
         <v>0.4</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F41" s="6" t="s">
         <v>34</v>
       </c>
       <c r="H41" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I41" s="6"/>
       <c r="J41" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K41" s="3">
         <v>1</v>
@@ -3797,7 +3789,7 @@
         <v>82</v>
       </c>
       <c r="V41" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.2">
@@ -3811,20 +3803,20 @@
         <v>0.4</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F42" s="6" t="s">
         <v>34</v>
       </c>
       <c r="H42" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I42" s="6"/>
       <c r="J42" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K42" s="3">
         <v>1</v>
@@ -3860,7 +3852,7 @@
         <v>82</v>
       </c>
       <c r="V42" s="6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -3875,8 +3867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3902,7 +3894,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
@@ -3914,16 +3906,16 @@
         <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>41</v>
@@ -3962,7 +3954,7 @@
         <v>14</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:22" s="1" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
@@ -3985,13 +3977,13 @@
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>24</v>
@@ -4030,12 +4022,12 @@
         <v>32</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B3" s="2">
         <v>100</v>
@@ -4044,19 +4036,19 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
       <c r="J3" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>53</v>
@@ -4101,19 +4093,19 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>53</v>
@@ -4158,7 +4150,7 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>54</v>
@@ -4206,7 +4198,7 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B6" s="6">
         <v>100</v>
@@ -4215,7 +4207,7 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>54</v>
@@ -4224,11 +4216,11 @@
         <v>42</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J6" s="4" t="s">
         <v>52</v>
@@ -4276,10 +4268,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>35</v>
@@ -4288,7 +4280,7 @@
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>53</v>
@@ -4333,10 +4325,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>34</v>
@@ -4345,7 +4337,7 @@
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>53</v>
@@ -4390,7 +4382,7 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>54</v>
@@ -4438,7 +4430,7 @@
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B10" s="6">
         <v>100</v>
@@ -4447,7 +4439,7 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>54</v>
@@ -4456,11 +4448,11 @@
         <v>42</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J10" s="4" t="s">
         <v>52</v>
@@ -4508,18 +4500,18 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
       <c r="J11" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="K11" s="3" t="s">
         <v>53</v>
@@ -4564,18 +4556,18 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
       <c r="J12" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="K12" s="3" t="s">
         <v>53</v>
@@ -4620,7 +4612,7 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>54</v>
@@ -4667,7 +4659,7 @@
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B14" s="6">
         <v>100</v>
@@ -4676,7 +4668,7 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>54</v>
@@ -4685,11 +4677,11 @@
         <v>42</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="H14" s="6"/>
       <c r="I14" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J14" s="4" t="s">
         <v>52</v>
@@ -4737,10 +4729,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>35</v>
@@ -4794,13 +4786,13 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D16" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="F16" s="6" t="s">
         <v>134</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>136</v>
       </c>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
@@ -4851,10 +4843,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>42</v>
@@ -4899,7 +4891,7 @@
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B18" s="6">
         <v>160</v>
@@ -4908,20 +4900,20 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>42</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="H18" s="6"/>
       <c r="I18" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J18" s="4" t="s">
         <v>52</v>
@@ -4969,10 +4961,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>35</v>
@@ -5026,10 +5018,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F20" s="6" t="s">
         <v>34</v>
@@ -5083,10 +5075,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>42</v>
@@ -5131,7 +5123,7 @@
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B22" s="6">
         <v>160</v>
@@ -5140,20 +5132,20 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>42</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="H22" s="6"/>
       <c r="I22" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J22" s="4" t="s">
         <v>52</v>
@@ -5201,10 +5193,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>35</v>
@@ -5258,13 +5250,13 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
@@ -5315,10 +5307,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F25" s="6" t="s">
         <v>42</v>
@@ -5363,7 +5355,7 @@
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B26" s="6">
         <v>160</v>
@@ -5372,20 +5364,20 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>42</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="H26" s="6"/>
       <c r="I26" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J26" s="4" t="s">
         <v>52</v>
@@ -5433,13 +5425,13 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>75</v>
+        <v>35</v>
       </c>
       <c r="G27" s="6"/>
       <c r="J27" s="4" t="s">
@@ -5488,13 +5480,13 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>74</v>
+        <v>34</v>
       </c>
       <c r="G28" s="6"/>
       <c r="J28" s="4" t="s">
@@ -5543,10 +5535,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>42</v>
@@ -5589,7 +5581,7 @@
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B30" s="6">
         <v>250</v>
@@ -5598,19 +5590,19 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F30" s="6" t="s">
         <v>42</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J30" s="4" t="s">
         <v>52</v>
@@ -5658,13 +5650,13 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D31" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E31" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="E31" s="6" t="s">
-        <v>186</v>
-      </c>
       <c r="F31" s="6" t="s">
-        <v>74</v>
+        <v>35</v>
       </c>
       <c r="G31" s="6"/>
       <c r="J31" s="4" t="s">
@@ -5713,13 +5705,13 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D32" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E32" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="E32" s="6" t="s">
-        <v>186</v>
-      </c>
       <c r="F32" s="6" t="s">
-        <v>74</v>
+        <v>34</v>
       </c>
       <c r="G32" s="6"/>
       <c r="J32" s="4" t="s">
@@ -5768,10 +5760,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F33" s="6" t="s">
         <v>42</v>
@@ -5814,7 +5806,7 @@
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B34" s="6">
         <v>250</v>
@@ -5823,19 +5815,19 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F34" s="6" t="s">
         <v>42</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I34" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J34" s="4" t="s">
         <v>52</v>
@@ -5883,13 +5875,13 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>74</v>
+        <v>35</v>
       </c>
       <c r="G35" s="6"/>
       <c r="I35" s="6"/>
@@ -5939,13 +5931,13 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>74</v>
+        <v>34</v>
       </c>
       <c r="G36" s="6"/>
       <c r="I36" s="6"/>
@@ -5995,10 +5987,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F37" s="6" t="s">
         <v>42</v>
@@ -6042,7 +6034,7 @@
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B38" s="6">
         <v>250</v>
@@ -6051,19 +6043,19 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F38" s="6" t="s">
         <v>42</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I38" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J38" s="4" t="s">
         <v>52</v>
@@ -6111,10 +6103,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>42</v>
@@ -6158,7 +6150,7 @@
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B40" s="6">
         <v>400</v>
@@ -6167,19 +6159,19 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F40" s="6" t="s">
         <v>42</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I40" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J40" s="4" t="s">
         <v>57</v>
@@ -6227,10 +6219,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F41" s="6" t="s">
         <v>42</v>
@@ -6274,7 +6266,7 @@
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B42" s="6">
         <v>400</v>
@@ -6283,19 +6275,19 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F42" s="6" t="s">
         <v>42</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I42" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J42" s="4" t="s">
         <v>57</v>
@@ -6343,10 +6335,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F43" s="6" t="s">
         <v>42</v>
@@ -6390,7 +6382,7 @@
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B44" s="6">
         <v>400</v>
@@ -6399,19 +6391,19 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F44" s="6" t="s">
         <v>42</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I44" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J44" s="4" t="s">
         <v>57</v>
@@ -6459,10 +6451,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F45" s="6" t="s">
         <v>42</v>
@@ -6506,7 +6498,7 @@
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B46" s="6">
         <v>630</v>
@@ -6515,19 +6507,19 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F46" s="6" t="s">
         <v>42</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I46" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J46" s="4" t="s">
         <v>57</v>
@@ -6575,10 +6567,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F47" s="6" t="s">
         <v>42</v>
@@ -6622,7 +6614,7 @@
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B48" s="6">
         <v>630</v>
@@ -6631,19 +6623,19 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F48" s="6" t="s">
         <v>42</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I48" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J48" s="4" t="s">
         <v>57</v>
@@ -6691,10 +6683,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F49" s="6" t="s">
         <v>42</v>
@@ -6738,7 +6730,7 @@
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B50" s="6">
         <v>630</v>
@@ -6747,19 +6739,19 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F50" s="6" t="s">
         <v>42</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I50" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J50" s="4" t="s">
         <v>57</v>
@@ -6811,7 +6803,7 @@
   <dimension ref="A1:U17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6835,7 +6827,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
@@ -6847,10 +6839,10 @@
         <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>17</v>
@@ -6892,7 +6884,7 @@
         <v>14</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="1" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
@@ -6915,7 +6907,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>16</v>
@@ -6957,7 +6949,7 @@
         <v>32</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
@@ -6971,7 +6963,7 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>63</v>
@@ -7027,7 +7019,7 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>63</v>
@@ -7083,7 +7075,7 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>63</v>
@@ -7139,7 +7131,7 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>69</v>
@@ -7195,7 +7187,7 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>69</v>
@@ -7251,7 +7243,7 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>69</v>
@@ -7307,10 +7299,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>42</v>
@@ -7363,10 +7355,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>42</v>
@@ -7419,10 +7411,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>42</v>
@@ -7475,7 +7467,7 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>72</v>
@@ -7531,7 +7523,7 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>72</v>
@@ -7587,7 +7579,7 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>72</v>
@@ -7653,7 +7645,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
@@ -7665,77 +7657,77 @@
   <sheetData>
     <row r="1" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>152</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C3" s="6"/>
       <c r="E3" s="6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -7743,22 +7735,22 @@
         <v>42</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E5" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="F5" s="6" t="s">
-        <v>142</v>
-      </c>
       <c r="G5" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>